<commit_message>
Rw Usage Update Report_12212023
Rw Usage Update Report_12212023
</commit_message>
<xml_diff>
--- a/System_2.1.7.xlsx
+++ b/System_2.1.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EB144B-9E8C-409D-9F44-8611CD5FC371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1880D52E-CD72-47A4-A2BD-6B37F4E2240A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -3500,7 +3500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="749">
+  <cellXfs count="747">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4831,6 +4831,9 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5406,15 +5409,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5707,8 +5701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5764,10 +5758,10 @@
       <c r="I2" s="415" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="562" t="s">
+      <c r="J2" s="563" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="563"/>
+      <c r="K2" s="564"/>
       <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
@@ -5777,14 +5771,14 @@
       <c r="N2" s="361" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="564" t="s">
+      <c r="O2" s="565" t="s">
         <v>384</v>
       </c>
-      <c r="P2" s="565"/>
-      <c r="Q2" s="566"/>
-      <c r="R2" s="566"/>
-      <c r="S2" s="566"/>
-      <c r="T2" s="567" t="s">
+      <c r="P2" s="566"/>
+      <c r="Q2" s="567"/>
+      <c r="R2" s="567"/>
+      <c r="S2" s="567"/>
+      <c r="T2" s="568" t="s">
         <v>385</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -5798,7 +5792,7 @@
       <c r="C3" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="559"/>
+      <c r="D3" s="560"/>
       <c r="E3" s="349"/>
       <c r="F3" s="271" t="s">
         <v>69</v>
@@ -5834,7 +5828,7 @@
       <c r="S3" s="24">
         <v>0</v>
       </c>
-      <c r="T3" s="568"/>
+      <c r="T3" s="569"/>
       <c r="U3" s="19" t="s">
         <v>586</v>
       </c>
@@ -5850,7 +5844,7 @@
       <c r="C4" s="168" t="s">
         <v>361</v>
       </c>
-      <c r="D4" s="560"/>
+      <c r="D4" s="561"/>
       <c r="E4" s="61"/>
       <c r="F4" s="371" t="s">
         <v>42</v>
@@ -5867,7 +5861,7 @@
       </c>
       <c r="O4" s="6"/>
       <c r="P4" s="321"/>
-      <c r="T4" s="568"/>
+      <c r="T4" s="569"/>
     </row>
     <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -5876,7 +5870,7 @@
       <c r="C5" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="561"/>
+      <c r="D5" s="562"/>
       <c r="F5" s="375" t="s">
         <v>42</v>
       </c>
@@ -5895,12 +5889,12 @@
         <v>520</v>
       </c>
       <c r="P5" s="321"/>
-      <c r="T5" s="568"/>
+      <c r="T5" s="569"/>
       <c r="U5" s="209" t="s">
         <v>228</v>
       </c>
       <c r="V5" s="19">
-        <v>6120</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5934,7 +5928,7 @@
       <c r="P6" s="321"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="6"/>
-      <c r="T6" s="568"/>
+      <c r="T6" s="569"/>
     </row>
     <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="214" t="s">
@@ -5974,7 +5968,7 @@
       <c r="S7" s="24">
         <v>1</v>
       </c>
-      <c r="T7" s="568"/>
+      <c r="T7" s="569"/>
     </row>
     <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -6003,7 +5997,7 @@
       <c r="P8" s="321"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="6"/>
-      <c r="T8" s="568"/>
+      <c r="T8" s="569"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -6045,7 +6039,7 @@
       <c r="S9" s="24">
         <v>1</v>
       </c>
-      <c r="T9" s="568"/>
+      <c r="T9" s="569"/>
     </row>
     <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -6075,7 +6069,7 @@
         <v>520</v>
       </c>
       <c r="P10" s="321"/>
-      <c r="T10" s="568"/>
+      <c r="T10" s="569"/>
     </row>
     <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -6117,12 +6111,12 @@
       <c r="S11" s="24">
         <v>1</v>
       </c>
-      <c r="T11" s="568"/>
+      <c r="T11" s="569"/>
       <c r="U11" s="209" t="s">
         <v>227</v>
       </c>
       <c r="V11" s="64">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6150,7 +6144,7 @@
       <c r="P12" s="321"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="142"/>
-      <c r="T12" s="568"/>
+      <c r="T12" s="569"/>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="261" t="s">
@@ -6182,7 +6176,7 @@
       </c>
       <c r="P13" s="321"/>
       <c r="R13" s="142"/>
-      <c r="T13" s="568"/>
+      <c r="T13" s="569"/>
       <c r="U13" s="2" t="s">
         <v>610</v>
       </c>
@@ -6192,7 +6186,7 @@
     </row>
     <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P14" s="321"/>
-      <c r="T14" s="568"/>
+      <c r="T14" s="569"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -6218,10 +6212,10 @@
       <c r="L15" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="556">
+      <c r="M15" s="557">
         <v>45275</v>
       </c>
-      <c r="N15" s="559" t="s">
+      <c r="N15" s="560" t="s">
         <v>22</v>
       </c>
       <c r="O15" s="500" t="s">
@@ -6239,7 +6233,7 @@
       <c r="S15" s="24">
         <v>1</v>
       </c>
-      <c r="T15" s="568"/>
+      <c r="T15" s="569"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="486" t="s">
@@ -6265,8 +6259,8 @@
       <c r="L16" s="199" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="557"/>
-      <c r="N16" s="560"/>
+      <c r="M16" s="558"/>
+      <c r="N16" s="561"/>
       <c r="P16" s="321">
         <v>1</v>
       </c>
@@ -6279,7 +6273,7 @@
       <c r="S16" s="112">
         <v>1</v>
       </c>
-      <c r="T16" s="568"/>
+      <c r="T16" s="569"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -6307,8 +6301,8 @@
       <c r="L17" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="M17" s="558"/>
-      <c r="N17" s="561"/>
+      <c r="M17" s="559"/>
+      <c r="N17" s="562"/>
       <c r="O17" s="500" t="s">
         <v>44</v>
       </c>
@@ -6324,11 +6318,11 @@
       <c r="S17" s="24">
         <v>0</v>
       </c>
-      <c r="T17" s="568"/>
+      <c r="T17" s="569"/>
     </row>
     <row r="18" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="P18" s="321"/>
-      <c r="T18" s="568"/>
+      <c r="T18" s="569"/>
     </row>
     <row r="19" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
@@ -6356,14 +6350,14 @@
       <c r="L19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="556">
+      <c r="M19" s="557">
         <v>45275</v>
       </c>
       <c r="N19" s="414" t="s">
         <v>520</v>
       </c>
       <c r="P19" s="321"/>
-      <c r="T19" s="568"/>
+      <c r="T19" s="569"/>
     </row>
     <row r="20" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="246" t="s">
@@ -6389,7 +6383,7 @@
       <c r="L20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M20" s="557"/>
+      <c r="M20" s="558"/>
       <c r="N20" s="404" t="s">
         <v>26</v>
       </c>
@@ -6405,7 +6399,7 @@
       <c r="S20" s="24">
         <v>1</v>
       </c>
-      <c r="T20" s="568"/>
+      <c r="T20" s="569"/>
     </row>
     <row r="21" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="246" t="s">
@@ -6431,7 +6425,7 @@
       <c r="L21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="557"/>
+      <c r="M21" s="558"/>
       <c r="N21" s="404" t="s">
         <v>18</v>
       </c>
@@ -6447,11 +6441,11 @@
       <c r="S21" s="24">
         <v>1</v>
       </c>
-      <c r="T21" s="568"/>
-      <c r="U21" s="554" t="s">
+      <c r="T21" s="569"/>
+      <c r="U21" s="555" t="s">
         <v>226</v>
       </c>
-      <c r="V21" s="555"/>
+      <c r="V21" s="556"/>
     </row>
     <row r="22" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="276" t="s">
@@ -6477,12 +6471,12 @@
       <c r="L22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M22" s="557"/>
+      <c r="M22" s="558"/>
       <c r="N22" s="384" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="321"/>
-      <c r="T22" s="568"/>
+      <c r="T22" s="569"/>
       <c r="X22" s="19" t="s">
         <v>621</v>
       </c>
@@ -6511,12 +6505,12 @@
       <c r="L23" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="557"/>
+      <c r="M23" s="558"/>
       <c r="N23" s="61" t="s">
         <v>521</v>
       </c>
       <c r="P23" s="321"/>
-      <c r="T23" s="568"/>
+      <c r="T23" s="569"/>
       <c r="U23" s="2" t="s">
         <v>619</v>
       </c>
@@ -6551,7 +6545,7 @@
       <c r="L24" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="557"/>
+      <c r="M24" s="558"/>
       <c r="N24" s="61" t="s">
         <v>26</v>
       </c>
@@ -6560,7 +6554,7 @@
       </c>
       <c r="P24" s="548"/>
       <c r="S24" s="80"/>
-      <c r="T24" s="568"/>
+      <c r="T24" s="569"/>
     </row>
     <row r="25" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
@@ -6588,7 +6582,7 @@
       <c r="L25" s="135" t="s">
         <v>35</v>
       </c>
-      <c r="M25" s="557"/>
+      <c r="M25" s="558"/>
       <c r="N25" s="61" t="s">
         <v>26</v>
       </c>
@@ -6604,7 +6598,7 @@
       <c r="S25" s="21">
         <v>0</v>
       </c>
-      <c r="T25" s="568"/>
+      <c r="T25" s="569"/>
       <c r="V25" s="19"/>
     </row>
     <row r="26" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6631,12 +6625,12 @@
       <c r="L26" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="557"/>
+      <c r="M26" s="558"/>
       <c r="N26" s="61" t="s">
         <v>522</v>
       </c>
       <c r="P26" s="321"/>
-      <c r="T26" s="568"/>
+      <c r="T26" s="569"/>
       <c r="V26" s="549" t="s">
         <v>620</v>
       </c>
@@ -6661,7 +6655,7 @@
       <c r="J27" s="411"/>
       <c r="K27" s="412"/>
       <c r="L27" s="413"/>
-      <c r="M27" s="557"/>
+      <c r="M27" s="558"/>
       <c r="N27" s="61"/>
       <c r="P27" s="321">
         <v>1</v>
@@ -6675,7 +6669,7 @@
       <c r="S27" s="24">
         <v>0</v>
       </c>
-      <c r="T27" s="568"/>
+      <c r="T27" s="569"/>
       <c r="W27" s="2" t="s">
         <v>602</v>
       </c>
@@ -6704,7 +6698,7 @@
       <c r="L28" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M28" s="558"/>
+      <c r="M28" s="559"/>
       <c r="N28" s="61" t="s">
         <v>522</v>
       </c>
@@ -6720,7 +6714,7 @@
       <c r="S28" s="21">
         <v>0</v>
       </c>
-      <c r="T28" s="569"/>
+      <c r="T28" s="570"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6742,7 +6736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
@@ -6810,7 +6804,7 @@
       <c r="P1" s="422" t="s">
         <v>407</v>
       </c>
-      <c r="Q1" s="573" t="s">
+      <c r="Q1" s="574" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6834,7 +6828,7 @@
       <c r="AA1" s="553" t="s">
         <v>454</v>
       </c>
-      <c r="AB1" s="580" t="s">
+      <c r="AB1" s="581" t="s">
         <v>617</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -6855,32 +6849,32 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="586">
+      <c r="A2" s="587">
         <f ca="1">TODAY()</f>
         <v>45281</v>
       </c>
-      <c r="B2" s="588" t="s">
+      <c r="B2" s="589" t="s">
         <v>388</v>
       </c>
-      <c r="C2" s="600" t="s">
+      <c r="C2" s="601" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="590" t="s">
+      <c r="D2" s="591" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="592" t="s">
+      <c r="E2" s="593" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="598" t="s">
+      <c r="G2" s="599" t="s">
         <v>380</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="577" t="s">
+      <c r="I2" s="578" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6904,7 +6898,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="574"/>
+      <c r="Q2" s="575"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>4</v>
@@ -6933,7 +6927,7 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="581"/>
+      <c r="AB2" s="582"/>
       <c r="AC2" s="35"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="495"/>
@@ -6941,14 +6935,14 @@
       <c r="AK2" s="495"/>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="587"/>
-      <c r="B3" s="589"/>
-      <c r="C3" s="601"/>
-      <c r="D3" s="591"/>
-      <c r="E3" s="593"/>
-      <c r="G3" s="599"/>
+      <c r="A3" s="588"/>
+      <c r="B3" s="590"/>
+      <c r="C3" s="602"/>
+      <c r="D3" s="592"/>
+      <c r="E3" s="594"/>
+      <c r="G3" s="600"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="578"/>
+      <c r="I3" s="579"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6967,7 +6961,7 @@
         <v>252</v>
       </c>
       <c r="X3" s="496"/>
-      <c r="AB3" s="581"/>
+      <c r="AB3" s="582"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>612</v>
@@ -6987,10 +6981,10 @@
         <v>389</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="594" t="s">
+      <c r="C4" s="595" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="578"/>
+      <c r="I4" s="579"/>
       <c r="R4" s="497" t="s">
         <v>612</v>
       </c>
@@ -7008,7 +7002,7 @@
       <c r="X4" s="496">
         <v>1</v>
       </c>
-      <c r="AB4" s="581"/>
+      <c r="AB4" s="582"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -7030,7 +7024,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="595"/>
+      <c r="C5" s="596"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -7040,13 +7034,13 @@
       <c r="F5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G5" s="559" t="s">
+      <c r="G5" s="560" t="s">
         <v>276</v>
       </c>
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="578"/>
+      <c r="I5" s="579"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -7075,7 +7069,7 @@
       <c r="V5" s="494"/>
       <c r="W5" s="6"/>
       <c r="X5" s="494"/>
-      <c r="AB5" s="581"/>
+      <c r="AB5" s="582"/>
       <c r="AC5" s="2" t="s">
         <v>615</v>
       </c>
@@ -7090,19 +7084,19 @@
       <c r="AK5" s="494"/>
     </row>
     <row r="6" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="583" t="s">
+      <c r="A6" s="584" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="596"/>
-      <c r="D6" s="597"/>
+      <c r="C6" s="597"/>
+      <c r="D6" s="598"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
-      <c r="G6" s="560"/>
-      <c r="I6" s="578"/>
+      <c r="G6" s="561"/>
+      <c r="I6" s="579"/>
       <c r="P6" s="61" t="s">
         <v>615</v>
       </c>
@@ -7114,7 +7108,7 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="581"/>
+      <c r="AB6" s="582"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AI1:AI10)+AE11</f>
@@ -7128,7 +7122,7 @@
       <c r="AK6" s="342"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="584"/>
+      <c r="A7" s="585"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -7138,8 +7132,8 @@
       <c r="D7" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="560"/>
-      <c r="I7" s="578"/>
+      <c r="G7" s="561"/>
+      <c r="I7" s="579"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -7175,7 +7169,7 @@
       <c r="X7" s="495">
         <v>1</v>
       </c>
-      <c r="AB7" s="581"/>
+      <c r="AB7" s="582"/>
       <c r="AC7" s="99" t="s">
         <v>616</v>
       </c>
@@ -7186,7 +7180,7 @@
         <f>8-AE11</f>
         <v>2</v>
       </c>
-      <c r="AF7" s="748">
+      <c r="AF7" s="301">
         <f>8-AF11</f>
         <v>1</v>
       </c>
@@ -7200,7 +7194,7 @@
       <c r="AK7" s="495"/>
     </row>
     <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="585"/>
+      <c r="A8" s="586"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -7208,8 +7202,8 @@
       <c r="E8" s="30">
         <v>3</v>
       </c>
-      <c r="G8" s="560"/>
-      <c r="I8" s="578"/>
+      <c r="G8" s="561"/>
+      <c r="I8" s="579"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6" t="s">
         <v>465</v>
@@ -7219,7 +7213,7 @@
       </c>
       <c r="W8" s="6"/>
       <c r="X8" s="492"/>
-      <c r="AB8" s="581"/>
+      <c r="AB8" s="582"/>
       <c r="AC8" s="551"/>
       <c r="AH8" s="6" t="s">
         <v>624</v>
@@ -7230,7 +7224,7 @@
       <c r="AJ8" s="6" t="s">
         <v>624</v>
       </c>
-      <c r="AK8" s="747">
+      <c r="AK8" s="496">
         <v>1</v>
       </c>
     </row>
@@ -7247,9 +7241,9 @@
       <c r="D9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="560"/>
+      <c r="G9" s="561"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="578"/>
+      <c r="I9" s="579"/>
       <c r="M9" s="19" t="s">
         <v>544</v>
       </c>
@@ -7259,7 +7253,7 @@
       </c>
       <c r="V9" s="24"/>
       <c r="X9" s="492"/>
-      <c r="AB9" s="581"/>
+      <c r="AB9" s="582"/>
       <c r="AC9" s="551"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
@@ -7280,8 +7274,8 @@
         <f>Boat!U8</f>
         <v>37</v>
       </c>
-      <c r="G10" s="560"/>
-      <c r="I10" s="578"/>
+      <c r="G10" s="561"/>
+      <c r="I10" s="579"/>
       <c r="J10" s="24" t="s">
         <v>380</v>
       </c>
@@ -7298,7 +7292,7 @@
       <c r="V10" s="496"/>
       <c r="W10" s="6"/>
       <c r="X10" s="492"/>
-      <c r="AB10" s="581"/>
+      <c r="AB10" s="582"/>
       <c r="AC10" s="551"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
@@ -7311,7 +7305,7 @@
       <c r="A11" s="99" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="559" t="s">
+      <c r="B11" s="560" t="s">
         <v>391</v>
       </c>
       <c r="C11" s="175" t="s">
@@ -7320,8 +7314,8 @@
       <c r="D11" s="222" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="560"/>
-      <c r="I11" s="578"/>
+      <c r="G11" s="561"/>
+      <c r="I11" s="579"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7347,13 +7341,13 @@
       <c r="S11" s="24">
         <v>0</v>
       </c>
-      <c r="U11" s="570" t="s">
+      <c r="U11" s="571" t="s">
         <v>578</v>
       </c>
-      <c r="V11" s="571"/>
-      <c r="W11" s="571"/>
-      <c r="X11" s="572"/>
-      <c r="AB11" s="582"/>
+      <c r="V11" s="572"/>
+      <c r="W11" s="572"/>
+      <c r="X11" s="573"/>
+      <c r="AB11" s="583"/>
       <c r="AC11" s="99" t="s">
         <v>618</v>
       </c>
@@ -7367,23 +7361,23 @@
         <v>7</v>
       </c>
       <c r="AG11" s="438"/>
-      <c r="AH11" s="570" t="s">
+      <c r="AH11" s="571" t="s">
         <v>578</v>
       </c>
-      <c r="AI11" s="571"/>
-      <c r="AJ11" s="571"/>
-      <c r="AK11" s="572"/>
+      <c r="AI11" s="572"/>
+      <c r="AJ11" s="572"/>
+      <c r="AK11" s="573"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="561"/>
+      <c r="B12" s="562"/>
       <c r="E12" s="234">
         <v>3</v>
       </c>
-      <c r="G12" s="560"/>
-      <c r="I12" s="578"/>
+      <c r="G12" s="561"/>
+      <c r="I12" s="579"/>
       <c r="J12" s="24" t="s">
         <v>535</v>
       </c>
@@ -7411,12 +7405,12 @@
       <c r="B13" s="221" t="s">
         <v>330</v>
       </c>
-      <c r="C13" s="559" t="s">
+      <c r="C13" s="560" t="s">
         <v>195</v>
       </c>
       <c r="D13" s="20"/>
-      <c r="G13" s="560"/>
-      <c r="I13" s="578"/>
+      <c r="G13" s="561"/>
+      <c r="I13" s="579"/>
       <c r="J13" s="108" t="s">
         <v>568</v>
       </c>
@@ -7446,7 +7440,7 @@
       <c r="B14" s="177" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="561"/>
+      <c r="C14" s="562"/>
       <c r="D14" s="209" t="s">
         <v>154</v>
       </c>
@@ -7456,11 +7450,11 @@
       <c r="F14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="G14" s="561"/>
+      <c r="G14" s="562"/>
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="578"/>
+      <c r="I14" s="579"/>
       <c r="U14" s="67" t="s">
         <v>81</v>
       </c>
@@ -7487,7 +7481,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="578"/>
+      <c r="I15" s="579"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7518,7 +7512,7 @@
       <c r="D16" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I16" s="578"/>
+      <c r="I16" s="579"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7562,7 +7556,7 @@
       <c r="G17" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I17" s="578"/>
+      <c r="I17" s="579"/>
       <c r="L17" s="2" t="s">
         <v>443</v>
       </c>
@@ -7580,13 +7574,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="578"/>
+      <c r="I18" s="579"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="575" t="s">
+      <c r="O18" s="576" t="s">
         <v>536</v>
       </c>
-      <c r="P18" s="576"/>
+      <c r="P18" s="577"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7612,7 +7606,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="578"/>
+      <c r="I19" s="579"/>
       <c r="M19" s="21" t="s">
         <v>442</v>
       </c>
@@ -7644,7 +7638,7 @@
       <c r="G20" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I20" s="578"/>
+      <c r="I20" s="579"/>
       <c r="K20" s="19" t="s">
         <v>439</v>
       </c>
@@ -7675,7 +7669,7 @@
       <c r="X20" s="494"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="578"/>
+      <c r="I21" s="579"/>
       <c r="M21" s="221" t="s">
         <v>421</v>
       </c>
@@ -7705,7 +7699,7 @@
       <c r="G22" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="I22" s="578"/>
+      <c r="I22" s="579"/>
       <c r="P22" s="99" t="s">
         <v>614</v>
       </c>
@@ -7720,7 +7714,7 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="578"/>
+      <c r="I23" s="579"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
         <v>5</v>
@@ -7737,7 +7731,7 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="578"/>
+      <c r="I24" s="579"/>
       <c r="U24" s="35"/>
       <c r="V24" s="540">
         <v>1</v>
@@ -7765,7 +7759,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="578"/>
+      <c r="I25" s="579"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7810,7 +7804,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="578"/>
+      <c r="I26" s="579"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7845,7 +7839,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="578"/>
+      <c r="I27" s="579"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7872,7 +7866,7 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="578"/>
+      <c r="I28" s="579"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
@@ -7894,7 +7888,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="579"/>
+      <c r="I29" s="580"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -8045,7 +8039,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="598" t="s">
+      <c r="I1" s="599" t="s">
         <v>377</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -8081,7 +8075,7 @@
       <c r="X1" s="454" t="s">
         <v>156</v>
       </c>
-      <c r="Y1" s="644" t="s">
+      <c r="Y1" s="645" t="s">
         <v>548</v>
       </c>
       <c r="Z1" s="430">
@@ -8106,7 +8100,7 @@
         <v>515</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="629"/>
+      <c r="AN1" s="630"/>
       <c r="AO1" s="350" t="s">
         <v>486</v>
       </c>
@@ -8115,23 +8109,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="653">
+      <c r="A2" s="654">
         <f ca="1">TODAY()</f>
         <v>45281</v>
       </c>
-      <c r="B2" s="655" t="s">
+      <c r="B2" s="656" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="600" t="s">
+      <c r="C2" s="601" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="657" t="s">
+      <c r="D2" s="658" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="602" t="s">
+      <c r="E2" s="603" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="610" t="s">
+      <c r="F2" s="611" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -8140,31 +8134,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="599"/>
+      <c r="I2" s="600"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="604" t="s">
+      <c r="K2" s="605" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="605"/>
-      <c r="M2" s="610" t="s">
+      <c r="L2" s="606"/>
+      <c r="M2" s="611" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="636" t="s">
+      <c r="O2" s="637" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="600" t="s">
+      <c r="Q2" s="601" t="s">
         <v>144</v>
       </c>
-      <c r="R2" s="559"/>
-      <c r="S2" s="623" t="s">
+      <c r="R2" s="560"/>
+      <c r="S2" s="624" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -8174,7 +8168,7 @@
       <c r="X2" s="455" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="645"/>
+      <c r="Y2" s="646"/>
       <c r="Z2" s="431">
         <v>1</v>
       </c>
@@ -8197,15 +8191,15 @@
         <v>480</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="630"/>
+      <c r="AN2" s="631"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="654"/>
-      <c r="B3" s="656"/>
-      <c r="C3" s="601"/>
-      <c r="D3" s="658"/>
-      <c r="E3" s="603"/>
-      <c r="F3" s="611"/>
+      <c r="A3" s="655"/>
+      <c r="B3" s="657"/>
+      <c r="C3" s="602"/>
+      <c r="D3" s="659"/>
+      <c r="E3" s="604"/>
+      <c r="F3" s="612"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -8224,17 +8218,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="611"/>
+      <c r="M3" s="612"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="637"/>
+      <c r="O3" s="638"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="601"/>
-      <c r="R3" s="561"/>
-      <c r="S3" s="625"/>
+      <c r="Q3" s="602"/>
+      <c r="R3" s="562"/>
+      <c r="S3" s="626"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -8242,7 +8236,7 @@
       <c r="X3" s="455" t="s">
         <v>158</v>
       </c>
-      <c r="Y3" s="645"/>
+      <c r="Y3" s="646"/>
       <c r="Z3" s="432">
         <v>1</v>
       </c>
@@ -8251,7 +8245,7 @@
       <c r="AC3" s="100" t="s">
         <v>497</v>
       </c>
-      <c r="AD3" s="620" t="s">
+      <c r="AD3" s="621" t="s">
         <v>472</v>
       </c>
       <c r="AE3" s="262"/>
@@ -8263,16 +8257,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="630"/>
+      <c r="AN3" s="631"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="669" t="s">
+      <c r="B4" s="670" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="600" t="s">
+      <c r="C4" s="601" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -8281,7 +8275,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="611"/>
+      <c r="F4" s="612"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -8298,11 +8292,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="611"/>
+      <c r="M4" s="612"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="637"/>
+      <c r="O4" s="638"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -8324,12 +8318,12 @@
       <c r="X4" s="455" t="s">
         <v>159</v>
       </c>
-      <c r="Y4" s="645"/>
+      <c r="Y4" s="646"/>
       <c r="Z4" s="433"/>
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="620"/>
+      <c r="AD4" s="621"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -8339,37 +8333,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="630"/>
+      <c r="AN4" s="631"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="598" t="s">
+      <c r="A5" s="599" t="s">
         <v>434</v>
       </c>
-      <c r="B5" s="670"/>
-      <c r="C5" s="601"/>
+      <c r="B5" s="671"/>
+      <c r="C5" s="602"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="611"/>
-      <c r="G5" s="661" t="s">
+      <c r="F5" s="612"/>
+      <c r="G5" s="662" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="661"/>
-      <c r="I5" s="661"/>
-      <c r="J5" s="661"/>
-      <c r="K5" s="661"/>
-      <c r="L5" s="662"/>
-      <c r="M5" s="611"/>
+      <c r="H5" s="662"/>
+      <c r="I5" s="662"/>
+      <c r="J5" s="662"/>
+      <c r="K5" s="662"/>
+      <c r="L5" s="663"/>
+      <c r="M5" s="612"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="637"/>
+      <c r="O5" s="638"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8377,7 +8371,7 @@
       <c r="X5" s="455" t="s">
         <v>160</v>
       </c>
-      <c r="Y5" s="645"/>
+      <c r="Y5" s="646"/>
       <c r="Z5" s="433">
         <v>1</v>
       </c>
@@ -8400,24 +8394,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="630"/>
+      <c r="AN5" s="631"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="599"/>
-      <c r="B6" s="667" t="s">
+      <c r="A6" s="600"/>
+      <c r="B6" s="668" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="596"/>
-      <c r="D6" s="597"/>
-      <c r="F6" s="611"/>
-      <c r="G6" s="663"/>
-      <c r="H6" s="663"/>
-      <c r="I6" s="663"/>
-      <c r="J6" s="663"/>
-      <c r="K6" s="663"/>
-      <c r="L6" s="664"/>
-      <c r="M6" s="611"/>
-      <c r="O6" s="637"/>
+      <c r="C6" s="597"/>
+      <c r="D6" s="598"/>
+      <c r="F6" s="612"/>
+      <c r="G6" s="664"/>
+      <c r="H6" s="664"/>
+      <c r="I6" s="664"/>
+      <c r="J6" s="664"/>
+      <c r="K6" s="664"/>
+      <c r="L6" s="665"/>
+      <c r="M6" s="612"/>
+      <c r="O6" s="638"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8427,7 +8421,7 @@
       <c r="X6" s="455" t="s">
         <v>161</v>
       </c>
-      <c r="Y6" s="645"/>
+      <c r="Y6" s="646"/>
       <c r="Z6" s="431">
         <v>1</v>
       </c>
@@ -8441,16 +8435,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="619"/>
+      <c r="AI6" s="620"/>
       <c r="AJ6" s="465" t="s">
         <v>475</v>
       </c>
-      <c r="AK6" s="619" t="s">
+      <c r="AK6" s="620" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="630"/>
+      <c r="AN6" s="631"/>
       <c r="AO6" s="350" t="s">
         <v>487</v>
       </c>
@@ -8459,7 +8453,7 @@
       <c r="A7" s="237" t="s">
         <v>593</v>
       </c>
-      <c r="B7" s="668"/>
+      <c r="B7" s="669"/>
       <c r="C7" s="207" t="s">
         <v>382</v>
       </c>
@@ -8469,7 +8463,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="611"/>
+      <c r="F7" s="612"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8482,14 +8476,14 @@
       <c r="J7" s="30">
         <v>0</v>
       </c>
-      <c r="K7" s="559">
+      <c r="K7" s="560">
         <v>0</v>
       </c>
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="611"/>
-      <c r="O7" s="637"/>
+      <c r="M7" s="612"/>
+      <c r="O7" s="638"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8503,7 +8497,7 @@
       <c r="X7" s="455" t="s">
         <v>162</v>
       </c>
-      <c r="Y7" s="645"/>
+      <c r="Y7" s="646"/>
       <c r="Z7" s="431">
         <v>1</v>
       </c>
@@ -8513,18 +8507,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="620" t="s">
+      <c r="AG7" s="621" t="s">
         <v>471</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="619"/>
+      <c r="AI7" s="620"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="619"/>
+      <c r="AK7" s="620"/>
       <c r="AL7" s="80" t="s">
         <v>513</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="630"/>
+      <c r="AN7" s="631"/>
       <c r="AP7" s="76" t="s">
         <v>488</v>
       </c>
@@ -8541,27 +8535,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="611"/>
-      <c r="G8" s="662">
-        <v>0</v>
-      </c>
-      <c r="H8" s="659" t="s">
+      <c r="F8" s="612"/>
+      <c r="G8" s="663">
+        <v>0</v>
+      </c>
+      <c r="H8" s="660" t="s">
         <v>105</v>
       </c>
-      <c r="I8" s="559">
-        <v>0</v>
-      </c>
-      <c r="J8" s="659" t="s">
+      <c r="I8" s="560">
+        <v>0</v>
+      </c>
+      <c r="J8" s="660" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="665"/>
-      <c r="L8" s="621"/>
-      <c r="M8" s="634"/>
-      <c r="N8" s="626">
+      <c r="K8" s="666"/>
+      <c r="L8" s="622"/>
+      <c r="M8" s="635"/>
+      <c r="N8" s="627">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="637"/>
+      <c r="O8" s="638"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8571,7 +8565,7 @@
       <c r="X8" s="455" t="s">
         <v>163</v>
       </c>
-      <c r="Y8" s="645"/>
+      <c r="Y8" s="646"/>
       <c r="Z8" s="433"/>
       <c r="AA8" s="313"/>
       <c r="AB8" s="214"/>
@@ -8579,14 +8573,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="620"/>
+      <c r="AG8" s="621"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="619"/>
+      <c r="AI8" s="620"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="630"/>
+      <c r="AN8" s="631"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8601,17 +8595,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="611"/>
-      <c r="G9" s="664"/>
-      <c r="H9" s="660"/>
-      <c r="I9" s="561"/>
-      <c r="J9" s="660"/>
-      <c r="K9" s="666"/>
-      <c r="L9" s="622"/>
-      <c r="M9" s="635"/>
-      <c r="N9" s="627"/>
-      <c r="O9" s="638"/>
-      <c r="S9" s="623" t="s">
+      <c r="F9" s="612"/>
+      <c r="G9" s="665"/>
+      <c r="H9" s="661"/>
+      <c r="I9" s="562"/>
+      <c r="J9" s="661"/>
+      <c r="K9" s="667"/>
+      <c r="L9" s="623"/>
+      <c r="M9" s="636"/>
+      <c r="N9" s="628"/>
+      <c r="O9" s="639"/>
+      <c r="S9" s="624" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8623,7 +8617,7 @@
       <c r="X9" s="455" t="s">
         <v>164</v>
       </c>
-      <c r="Y9" s="645"/>
+      <c r="Y9" s="646"/>
       <c r="Z9" s="434"/>
       <c r="AA9" s="313"/>
       <c r="AB9" s="214"/>
@@ -8633,16 +8627,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="620"/>
+      <c r="AG9" s="621"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="619"/>
+      <c r="AI9" s="620"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="619" t="s">
+      <c r="AK9" s="620" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="630"/>
+      <c r="AN9" s="631"/>
       <c r="AP9" s="2" t="s">
         <v>525</v>
       </c>
@@ -8659,20 +8653,20 @@
         <f>Boat!U8</f>
         <v>37</v>
       </c>
-      <c r="F10" s="611"/>
+      <c r="F10" s="612"/>
       <c r="N10" s="442" t="s">
         <v>406</v>
       </c>
-      <c r="O10" s="613" t="s">
+      <c r="O10" s="614" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="639" t="s">
+      <c r="P10" s="640" t="s">
         <v>410</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="624"/>
+      <c r="S10" s="625"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8684,7 +8678,7 @@
       <c r="X10" s="455" t="s">
         <v>165</v>
       </c>
-      <c r="Y10" s="645"/>
+      <c r="Y10" s="646"/>
       <c r="Z10" s="433">
         <v>0</v>
       </c>
@@ -8702,16 +8696,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="620"/>
+      <c r="AG10" s="621"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="619"/>
+      <c r="AI10" s="620"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="619"/>
+      <c r="AK10" s="620"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="630"/>
+      <c r="AN10" s="631"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8720,7 +8714,7 @@
       <c r="A11" s="228" t="s">
         <v>290</v>
       </c>
-      <c r="B11" s="559" t="s">
+      <c r="B11" s="560" t="s">
         <v>288</v>
       </c>
       <c r="C11" s="481" t="s">
@@ -8729,18 +8723,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="611"/>
+      <c r="F11" s="612"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="614"/>
-      <c r="P11" s="640"/>
+      <c r="O11" s="615"/>
+      <c r="P11" s="641"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="624"/>
+      <c r="S11" s="625"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8750,7 +8744,7 @@
       <c r="X11" s="455" t="s">
         <v>166</v>
       </c>
-      <c r="Y11" s="645"/>
+      <c r="Y11" s="646"/>
       <c r="Z11" s="433"/>
       <c r="AA11" s="313">
         <v>1</v>
@@ -8764,14 +8758,14 @@
       <c r="AF11" s="262" t="s">
         <v>493</v>
       </c>
-      <c r="AG11" s="620"/>
+      <c r="AG11" s="621"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="630"/>
+      <c r="AN11" s="631"/>
       <c r="AP11" s="76" t="s">
         <v>501</v>
       </c>
@@ -8780,7 +8774,7 @@
       <c r="A12" s="232" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="561"/>
+      <c r="B12" s="562"/>
       <c r="C12" s="482" t="s">
         <v>393</v>
       </c>
@@ -8790,25 +8784,25 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="611"/>
+      <c r="F12" s="612"/>
       <c r="G12" s="349" t="s">
         <v>410</v>
       </c>
-      <c r="H12" s="564" t="s">
+      <c r="H12" s="565" t="s">
         <v>446</v>
       </c>
-      <c r="I12" s="566"/>
-      <c r="J12" s="566"/>
-      <c r="K12" s="618"/>
+      <c r="I12" s="567"/>
+      <c r="J12" s="567"/>
+      <c r="K12" s="619"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="614"/>
-      <c r="P12" s="640"/>
+      <c r="O12" s="615"/>
+      <c r="P12" s="641"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="625"/>
+      <c r="S12" s="626"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8818,7 +8812,7 @@
       <c r="X12" s="455" t="s">
         <v>167</v>
       </c>
-      <c r="Y12" s="645"/>
+      <c r="Y12" s="646"/>
       <c r="Z12" s="431">
         <v>1</v>
       </c>
@@ -8829,16 +8823,16 @@
       <c r="AC12" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD12" s="628" t="s">
+      <c r="AD12" s="629" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="620" t="s">
+      <c r="AF12" s="621" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="620"/>
+      <c r="AG12" s="621"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8848,10 +8842,10 @@
       <c r="AJ12" s="262"/>
       <c r="AK12" s="262"/>
       <c r="AL12" s="262"/>
-      <c r="AM12" s="642" t="s">
+      <c r="AM12" s="643" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="630"/>
+      <c r="AN12" s="631"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8863,17 +8857,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="611"/>
-      <c r="G13" s="566" t="s">
+      <c r="F13" s="612"/>
+      <c r="G13" s="567" t="s">
         <v>447</v>
       </c>
-      <c r="H13" s="566"/>
-      <c r="I13" s="566"/>
-      <c r="J13" s="618"/>
+      <c r="H13" s="567"/>
+      <c r="I13" s="567"/>
+      <c r="J13" s="619"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="614"/>
-      <c r="P13" s="641"/>
+      <c r="O13" s="615"/>
+      <c r="P13" s="642"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8883,7 +8877,7 @@
       <c r="X13" s="455" t="s">
         <v>168</v>
       </c>
-      <c r="Y13" s="645"/>
+      <c r="Y13" s="646"/>
       <c r="Z13" s="431">
         <v>1</v>
       </c>
@@ -8894,8 +8888,8 @@
         <v>517</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="628"/>
-      <c r="AF13" s="620"/>
+      <c r="AD13" s="629"/>
+      <c r="AF13" s="621"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8906,8 +8900,8 @@
       <c r="AJ13" s="80"/>
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
-      <c r="AM13" s="642"/>
-      <c r="AN13" s="630"/>
+      <c r="AM13" s="643"/>
+      <c r="AN13" s="631"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8915,18 +8909,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="611"/>
-      <c r="G14" s="566" t="s">
+      <c r="F14" s="612"/>
+      <c r="G14" s="567" t="s">
         <v>446</v>
       </c>
-      <c r="H14" s="566"/>
-      <c r="I14" s="566"/>
-      <c r="J14" s="618"/>
+      <c r="H14" s="567"/>
+      <c r="I14" s="567"/>
+      <c r="J14" s="619"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="614"/>
+      <c r="O14" s="615"/>
       <c r="Q14" s="61" t="s">
         <v>552</v>
       </c>
@@ -8940,34 +8934,34 @@
       <c r="X14" s="455" t="s">
         <v>169</v>
       </c>
-      <c r="Y14" s="645"/>
+      <c r="Y14" s="646"/>
       <c r="Z14" s="431">
         <v>1</v>
       </c>
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="628"/>
+      <c r="AD14" s="629"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="620"/>
+      <c r="AF14" s="621"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
       <c r="AJ14" s="262"/>
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
-      <c r="AM14" s="642"/>
-      <c r="AN14" s="630"/>
+      <c r="AM14" s="643"/>
+      <c r="AN14" s="631"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
         <v>523</v>
       </c>
-      <c r="C15" s="559" t="s">
+      <c r="C15" s="560" t="s">
         <v>381</v>
       </c>
-      <c r="F15" s="611"/>
-      <c r="O15" s="614"/>
+      <c r="F15" s="612"/>
+      <c r="O15" s="615"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8980,7 +8974,7 @@
       <c r="X15" s="455" t="s">
         <v>170</v>
       </c>
-      <c r="Y15" s="645"/>
+      <c r="Y15" s="646"/>
       <c r="Z15" s="433">
         <v>1</v>
       </c>
@@ -8989,8 +8983,8 @@
       <c r="AC15" s="76" t="s">
         <v>496</v>
       </c>
-      <c r="AD15" s="628"/>
-      <c r="AF15" s="620"/>
+      <c r="AD15" s="629"/>
+      <c r="AF15" s="621"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>465</v>
@@ -9003,8 +8997,8 @@
       </c>
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
-      <c r="AM15" s="642"/>
-      <c r="AN15" s="630"/>
+      <c r="AM15" s="643"/>
+      <c r="AN15" s="631"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -9019,20 +9013,20 @@
       <c r="B16" s="21" t="s">
         <v>416</v>
       </c>
-      <c r="C16" s="561"/>
+      <c r="C16" s="562"/>
       <c r="D16" s="61" t="s">
         <v>510</v>
       </c>
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="611"/>
+      <c r="F16" s="612"/>
       <c r="G16" s="349" t="s">
         <v>505</v>
       </c>
       <c r="I16" s="495"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="614"/>
+      <c r="O16" s="615"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -9043,7 +9037,7 @@
       <c r="X16" s="455" t="s">
         <v>171</v>
       </c>
-      <c r="Y16" s="645"/>
+      <c r="Y16" s="646"/>
       <c r="Z16" s="431">
         <v>1</v>
       </c>
@@ -9064,18 +9058,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="630"/>
+      <c r="AN16" s="631"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="611"/>
+      <c r="F17" s="612"/>
       <c r="I17" s="496"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="614"/>
+      <c r="O17" s="615"/>
       <c r="Q17" s="21" t="s">
         <v>550</v>
       </c>
@@ -9095,7 +9089,7 @@
       <c r="X17" s="455" t="s">
         <v>172</v>
       </c>
-      <c r="Y17" s="645"/>
+      <c r="Y17" s="646"/>
       <c r="Z17" s="433"/>
       <c r="AA17" s="313"/>
       <c r="AB17" s="214"/>
@@ -9120,7 +9114,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="630"/>
+      <c r="AN17" s="631"/>
       <c r="AO17" s="209" t="s">
         <v>514</v>
       </c>
@@ -9144,21 +9138,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="611"/>
+      <c r="F18" s="612"/>
       <c r="G18" s="349" t="s">
         <v>547</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="614"/>
+      <c r="O18" s="615"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="606" t="s">
+      <c r="R18" s="607" t="s">
         <v>555</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="650" t="s">
+      <c r="U18" s="651" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -9168,7 +9162,7 @@
       <c r="X18" s="455" t="s">
         <v>173</v>
       </c>
-      <c r="Y18" s="645"/>
+      <c r="Y18" s="646"/>
       <c r="Z18" s="433">
         <v>1</v>
       </c>
@@ -9179,38 +9173,38 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="619" t="s">
+      <c r="AF18" s="620" t="s">
         <v>492</v>
       </c>
       <c r="AG18" s="262"/>
       <c r="AH18" s="70"/>
       <c r="AI18" s="70"/>
-      <c r="AJ18" s="643" t="s">
+      <c r="AJ18" s="644" t="s">
         <v>322</v>
       </c>
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="630"/>
+      <c r="AN18" s="631"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="611"/>
+      <c r="F19" s="612"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="614"/>
-      <c r="R19" s="607"/>
+      <c r="O19" s="615"/>
+      <c r="R19" s="608"/>
       <c r="S19" s="30" t="s">
         <v>553</v>
       </c>
-      <c r="U19" s="651"/>
+      <c r="U19" s="652"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
         <v>174</v>
       </c>
-      <c r="Y19" s="645"/>
+      <c r="Y19" s="646"/>
       <c r="Z19" s="431">
         <v>1</v>
       </c>
@@ -9219,17 +9213,17 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="619"/>
+      <c r="AF19" s="620"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
-      <c r="AJ19" s="643"/>
+      <c r="AJ19" s="644"/>
       <c r="AK19" s="484" t="s">
         <v>256</v>
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="630"/>
+      <c r="AN19" s="631"/>
       <c r="AP19" s="76" t="s">
         <v>485</v>
       </c>
@@ -9250,24 +9244,24 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="611"/>
+      <c r="F20" s="612"/>
       <c r="G20" s="349" t="s">
         <v>508</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="614"/>
-      <c r="Q20" s="616" t="s">
+      <c r="O20" s="615"/>
+      <c r="Q20" s="617" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="652"/>
+      <c r="U20" s="653"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
       </c>
-      <c r="Y20" s="645"/>
+      <c r="Y20" s="646"/>
       <c r="Z20" s="435">
         <v>1</v>
       </c>
@@ -9292,7 +9286,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="630"/>
+      <c r="AN20" s="631"/>
       <c r="AO20" s="350" t="s">
         <v>477</v>
       </c>
@@ -9313,20 +9307,20 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="611"/>
+      <c r="F21" s="612"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="614"/>
-      <c r="Q21" s="617"/>
+      <c r="O21" s="615"/>
+      <c r="Q21" s="618"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="647"/>
+      <c r="V21" s="648"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X21" s="453" t="s">
         <v>187</v>
       </c>
-      <c r="Y21" s="645"/>
+      <c r="Y21" s="646"/>
       <c r="Z21" s="469">
         <v>3</v>
       </c>
@@ -9357,15 +9351,15 @@
       <c r="AM21" s="452" t="s">
         <v>564</v>
       </c>
-      <c r="AN21" s="630"/>
+      <c r="AN21" s="631"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="611"/>
+      <c r="F22" s="612"/>
       <c r="G22" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="614"/>
+      <c r="O22" s="615"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9373,14 +9367,14 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="648"/>
+      <c r="V22" s="649"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
       <c r="X22" s="453" t="s">
         <v>188</v>
       </c>
-      <c r="Y22" s="645"/>
+      <c r="Y22" s="646"/>
       <c r="Z22" s="439"/>
       <c r="AA22" s="10"/>
       <c r="AB22" s="439"/>
@@ -9391,7 +9385,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="619" t="s">
+      <c r="AJ22" s="620" t="s">
         <v>489</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9399,7 +9393,7 @@
         <v>495</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="630"/>
+      <c r="AN22" s="631"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9417,22 +9411,22 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="611"/>
+      <c r="F23" s="612"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="614"/>
-      <c r="Q23" s="616" t="s">
+      <c r="O23" s="615"/>
+      <c r="Q23" s="617" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="648"/>
+      <c r="V23" s="649"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
       </c>
-      <c r="Y23" s="645"/>
+      <c r="Y23" s="646"/>
       <c r="Z23" s="17"/>
       <c r="AA23" s="10"/>
       <c r="AB23" s="439"/>
@@ -9443,13 +9437,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="619"/>
+      <c r="AJ23" s="620"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>524</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="630"/>
+      <c r="AN23" s="631"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9467,23 +9461,23 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="611"/>
+      <c r="F24" s="612"/>
       <c r="G24" s="61" t="s">
         <v>507</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="614"/>
-      <c r="Q24" s="617"/>
+      <c r="O24" s="615"/>
+      <c r="Q24" s="618"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="648"/>
+      <c r="V24" s="649"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
       </c>
-      <c r="Y24" s="645"/>
+      <c r="Y24" s="646"/>
       <c r="Z24" s="17"/>
       <c r="AA24" s="10"/>
       <c r="AB24" s="439"/>
@@ -9502,12 +9496,12 @@
         <v>480</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="630"/>
+      <c r="AN24" s="631"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="611"/>
+      <c r="F25" s="612"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="614"/>
+      <c r="O25" s="615"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9520,12 +9514,12 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="649"/>
+      <c r="V25" s="650"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
       </c>
-      <c r="Y25" s="645"/>
+      <c r="Y25" s="646"/>
       <c r="Z25" s="17"/>
       <c r="AA25" s="10"/>
       <c r="AB25" s="439"/>
@@ -9542,7 +9536,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="630"/>
+      <c r="AN25" s="631"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9560,17 +9554,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="611"/>
+      <c r="F26" s="612"/>
       <c r="G26" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="614"/>
-      <c r="P26" s="632" t="s">
+      <c r="O26" s="615"/>
+      <c r="P26" s="633" t="s">
         <v>545</v>
       </c>
-      <c r="Q26" s="633"/>
-      <c r="R26" s="608" t="s">
+      <c r="Q26" s="634"/>
+      <c r="R26" s="609" t="s">
         <v>554</v>
       </c>
       <c r="T26" s="182"/>
@@ -9582,7 +9576,7 @@
       <c r="X26" s="453" t="s">
         <v>182</v>
       </c>
-      <c r="Y26" s="645"/>
+      <c r="Y26" s="646"/>
       <c r="Z26" s="17"/>
       <c r="AA26" s="10"/>
       <c r="AB26" s="439"/>
@@ -9609,7 +9603,7 @@
       <c r="AM26" s="466" t="s">
         <v>473</v>
       </c>
-      <c r="AN26" s="630"/>
+      <c r="AN26" s="631"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9621,13 +9615,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="612"/>
+      <c r="F27" s="613"/>
       <c r="G27" s="61" t="s">
         <v>563</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="615"/>
-      <c r="R27" s="609"/>
+      <c r="O27" s="616"/>
+      <c r="R27" s="610"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9640,7 +9634,7 @@
       <c r="X27" s="453" t="s">
         <v>549</v>
       </c>
-      <c r="Y27" s="646"/>
+      <c r="Y27" s="647"/>
       <c r="Z27" s="163"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="440"/>
@@ -9657,7 +9651,7 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="631"/>
+      <c r="AN27" s="632"/>
     </row>
   </sheetData>
   <mergeCells count="54">
@@ -9724,7 +9718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N18" workbookViewId="0">
+    <sheetView topLeftCell="N18" workbookViewId="0">
       <selection activeCell="AN27" sqref="AN27"/>
     </sheetView>
   </sheetViews>
@@ -9820,10 +9814,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="674" t="s">
+      <c r="V1" s="675" t="s">
         <v>458</v>
       </c>
-      <c r="W1" s="675"/>
+      <c r="W1" s="676"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9839,21 +9833,21 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="676" t="s">
+      <c r="AC1" s="677" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="677"/>
-      <c r="AE1" s="678"/>
-      <c r="AF1" s="679" t="s">
+      <c r="AD1" s="678"/>
+      <c r="AE1" s="679"/>
+      <c r="AF1" s="680" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="680"/>
-      <c r="AH1" s="681"/>
-      <c r="AI1" s="671" t="s">
+      <c r="AG1" s="681"/>
+      <c r="AH1" s="682"/>
+      <c r="AI1" s="672" t="s">
         <v>461</v>
       </c>
-      <c r="AJ1" s="672"/>
-      <c r="AK1" s="673"/>
+      <c r="AJ1" s="673"/>
+      <c r="AK1" s="674"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9870,19 +9864,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="682">
+      <c r="L2" s="683">
         <f>SUM(L5:L30)</f>
         <v>1</v>
       </c>
-      <c r="M2" s="684">
+      <c r="M2" s="685">
         <f>SUM(M4:M29)</f>
         <v>11</v>
       </c>
-      <c r="N2" s="686">
+      <c r="N2" s="687">
         <f>SUM(N4:N29)</f>
         <v>10</v>
       </c>
-      <c r="O2" s="626">
+      <c r="O2" s="627">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9901,7 +9895,7 @@
       <c r="T2" s="509" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="688" t="s">
+      <c r="U2" s="689" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="510" t="s">
@@ -9970,10 +9964,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="683"/>
-      <c r="M3" s="685"/>
-      <c r="N3" s="687"/>
-      <c r="O3" s="627"/>
+      <c r="L3" s="684"/>
+      <c r="M3" s="686"/>
+      <c r="N3" s="688"/>
+      <c r="O3" s="628"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9989,7 +9983,7 @@
         <f>SUM(T4:T29)</f>
         <v>37</v>
       </c>
-      <c r="U3" s="689"/>
+      <c r="U3" s="690"/>
       <c r="V3" s="513">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>6</v>
@@ -10088,7 +10082,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="691" t="s">
+      <c r="O4" s="692" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -10167,7 +10161,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="692"/>
+      <c r="O5" s="693"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -10254,7 +10248,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="692"/>
+      <c r="O6" s="693"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
@@ -10348,7 +10342,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="692"/>
+      <c r="O7" s="693"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10456,7 +10450,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="692"/>
+      <c r="O8" s="693"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10540,7 +10534,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="692"/>
+      <c r="O9" s="693"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
@@ -10634,7 +10628,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="692"/>
+      <c r="O10" s="693"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10717,7 +10711,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="692"/>
+      <c r="O11" s="693"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10777,7 +10771,7 @@
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="662" t="s">
+      <c r="A12" s="663" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10786,7 +10780,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="616" t="s">
+      <c r="E12" s="617" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
@@ -10807,7 +10801,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="692"/>
+      <c r="O12" s="693"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10879,14 +10873,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="664"/>
+      <c r="A13" s="665"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="617"/>
+      <c r="E13" s="618"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10909,7 +10903,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="692"/>
+      <c r="O13" s="693"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10985,7 +10979,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="O14" s="692"/>
+      <c r="O14" s="693"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -11080,7 +11074,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="692"/>
+      <c r="O15" s="693"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -11167,7 +11161,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="692"/>
+      <c r="O16" s="693"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -11265,7 +11259,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="692"/>
+      <c r="O17" s="693"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -11360,7 +11354,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="692"/>
+      <c r="O18" s="693"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11443,7 +11437,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="692"/>
+      <c r="O19" s="693"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11543,11 +11537,11 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="693"/>
-      <c r="P20" s="564" t="s">
+      <c r="O20" s="694"/>
+      <c r="P20" s="565" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="618"/>
+      <c r="Q20" s="619"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
@@ -11783,7 +11777,7 @@
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="669" t="s">
+      <c r="E23" s="670" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11879,7 +11873,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="670"/>
+      <c r="E24" s="671"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
@@ -11897,10 +11891,10 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P24" s="564" t="s">
+      <c r="P24" s="565" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="618"/>
+      <c r="Q24" s="619"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
@@ -12496,10 +12490,10 @@
       <c r="H32">
         <v>-1</v>
       </c>
-      <c r="I32" s="665" t="s">
+      <c r="I32" s="666" t="s">
         <v>608</v>
       </c>
-      <c r="J32" s="690"/>
+      <c r="J32" s="691"/>
       <c r="K32" s="406"/>
       <c r="L32" s="544">
         <v>0</v>
@@ -12833,7 +12827,7 @@
       <c r="M36" s="255">
         <v>0</v>
       </c>
-      <c r="N36" s="746">
+      <c r="N36" s="554">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -13044,15 +13038,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="564" t="s">
+      <c r="B1" s="565" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="618"/>
+      <c r="C1" s="619"/>
       <c r="D1" s="209"/>
-      <c r="J1" s="564" t="s">
+      <c r="J1" s="565" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="618"/>
+      <c r="K1" s="619"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13090,13 +13084,13 @@
         <v>34</v>
       </c>
       <c r="L2" s="201"/>
-      <c r="M2" s="694"/>
+      <c r="M2" s="695"/>
       <c r="N2" s="154">
         <v>2</v>
       </c>
       <c r="O2" s="155"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="697" t="s">
+      <c r="Q2" s="698" t="s">
         <v>44</v>
       </c>
       <c r="R2" s="19">
@@ -13119,13 +13113,13 @@
       <c r="K3" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="M3" s="695"/>
+      <c r="M3" s="696"/>
       <c r="N3" s="17">
         <v>1</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="698"/>
+      <c r="Q3" s="699"/>
       <c r="R3" s="224"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13144,13 +13138,13 @@
       <c r="K4" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="M4" s="695"/>
+      <c r="M4" s="696"/>
       <c r="N4" s="17"/>
       <c r="O4" s="15">
         <v>1</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="698"/>
+      <c r="Q4" s="699"/>
       <c r="R4" s="224"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13170,13 +13164,13 @@
         <v>13</v>
       </c>
       <c r="L5" s="201"/>
-      <c r="M5" s="695"/>
+      <c r="M5" s="696"/>
       <c r="N5" s="17">
         <v>1</v>
       </c>
       <c r="O5" s="15"/>
       <c r="P5" s="10"/>
-      <c r="Q5" s="698"/>
+      <c r="Q5" s="699"/>
       <c r="R5" s="19">
         <v>-1</v>
       </c>
@@ -13197,13 +13191,13 @@
       <c r="K6" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="M6" s="695"/>
+      <c r="M6" s="696"/>
       <c r="N6" s="17">
         <v>1</v>
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="10"/>
-      <c r="Q6" s="698"/>
+      <c r="Q6" s="699"/>
       <c r="R6" s="224"/>
     </row>
     <row r="7" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13223,13 +13217,13 @@
         <v>334</v>
       </c>
       <c r="L7" s="203"/>
-      <c r="M7" s="695"/>
+      <c r="M7" s="696"/>
       <c r="N7" s="17">
         <v>1</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="10"/>
-      <c r="Q7" s="698"/>
+      <c r="Q7" s="699"/>
       <c r="R7" s="19">
         <v>-1</v>
       </c>
@@ -13250,13 +13244,13 @@
       <c r="K8" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="M8" s="695"/>
+      <c r="M8" s="696"/>
       <c r="N8" s="17">
         <v>1</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="698"/>
+      <c r="Q8" s="699"/>
       <c r="R8" s="224"/>
     </row>
     <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13276,13 +13270,13 @@
         <v>336</v>
       </c>
       <c r="L9" s="185"/>
-      <c r="M9" s="696"/>
+      <c r="M9" s="697"/>
       <c r="N9" s="163"/>
       <c r="O9" s="18"/>
       <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="Q9" s="699"/>
+      <c r="Q9" s="700"/>
       <c r="R9" s="225"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
@@ -13440,10 +13434,10 @@
         <f ca="1">TODAY()</f>
         <v>45281</v>
       </c>
-      <c r="V1" s="564" t="s">
+      <c r="V1" s="565" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="618"/>
+      <c r="W1" s="619"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13462,7 +13456,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="707" t="s">
+      <c r="AD1" s="708" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13479,10 +13473,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="706" t="s">
+      <c r="F2" s="707" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="734" t="s">
+      <c r="G2" s="735" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13510,10 +13504,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="674" t="s">
+      <c r="V2" s="675" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="675"/>
+      <c r="W2" s="676"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13532,7 +13526,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="708"/>
+      <c r="AD2" s="709"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13551,8 +13545,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="666"/>
-      <c r="G3" s="735"/>
+      <c r="F3" s="667"/>
+      <c r="G3" s="736"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13563,13 +13557,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="744" t="s">
+      <c r="O3" s="745" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="726" t="s">
+      <c r="P3" s="727" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="727"/>
+      <c r="Q3" s="728"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13579,15 +13573,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="708"/>
+      <c r="AD3" s="709"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="735"/>
+      <c r="G4" s="736"/>
       <c r="H4" s="6"/>
-      <c r="L4" s="697" t="s">
+      <c r="L4" s="698" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="745"/>
+      <c r="O4" s="746"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13597,12 +13591,12 @@
       <c r="X4" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="Y4" s="564" t="s">
+      <c r="Y4" s="565" t="s">
         <v>195</v>
       </c>
-      <c r="Z4" s="566"/>
-      <c r="AA4" s="618"/>
-      <c r="AD4" s="708"/>
+      <c r="Z4" s="567"/>
+      <c r="AA4" s="619"/>
+      <c r="AD4" s="709"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13617,21 +13611,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="735"/>
+      <c r="G5" s="736"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="713" t="s">
+      <c r="K5" s="714" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="728"/>
+      <c r="L5" s="729"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="745"/>
+      <c r="O5" s="746"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13647,11 +13641,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="716" t="s">
+      <c r="Y5" s="717" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="717"/>
-      <c r="AD5" s="708"/>
+      <c r="Z5" s="718"/>
+      <c r="AD5" s="709"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13661,16 +13655,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="735"/>
+      <c r="G6" s="736"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="714"/>
-      <c r="L6" s="728"/>
-      <c r="O6" s="745"/>
+      <c r="K6" s="715"/>
+      <c r="L6" s="729"/>
+      <c r="O6" s="746"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13680,23 +13674,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="708"/>
+      <c r="AD6" s="709"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="735"/>
+      <c r="G7" s="736"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="714"/>
-      <c r="L7" s="728"/>
+      <c r="K7" s="715"/>
+      <c r="L7" s="729"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="745"/>
+      <c r="O7" s="746"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="708"/>
+      <c r="AD7" s="709"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13709,7 +13703,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="735"/>
+      <c r="G8" s="736"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13719,41 +13713,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="714"/>
-      <c r="L8" s="728"/>
-      <c r="O8" s="745"/>
+      <c r="K8" s="715"/>
+      <c r="L8" s="729"/>
+      <c r="O8" s="746"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="710" t="s">
+      <c r="S8" s="711" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="711"/>
-      <c r="U8" s="711"/>
-      <c r="V8" s="711"/>
-      <c r="W8" s="711"/>
-      <c r="X8" s="711"/>
-      <c r="Y8" s="711"/>
-      <c r="Z8" s="711"/>
-      <c r="AA8" s="711"/>
-      <c r="AB8" s="711"/>
-      <c r="AC8" s="712"/>
-      <c r="AD8" s="708"/>
+      <c r="T8" s="712"/>
+      <c r="U8" s="712"/>
+      <c r="V8" s="712"/>
+      <c r="W8" s="712"/>
+      <c r="X8" s="712"/>
+      <c r="Y8" s="712"/>
+      <c r="Z8" s="712"/>
+      <c r="AA8" s="712"/>
+      <c r="AB8" s="712"/>
+      <c r="AC8" s="713"/>
+      <c r="AD8" s="709"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="700"/>
-      <c r="G9" s="735"/>
+      <c r="C9" s="701"/>
+      <c r="G9" s="736"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="714"/>
-      <c r="L9" s="738" t="s">
+      <c r="K9" s="715"/>
+      <c r="L9" s="739" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="739"/>
-      <c r="N9" s="740"/>
-      <c r="O9" s="745"/>
+      <c r="M9" s="740"/>
+      <c r="N9" s="741"/>
+      <c r="O9" s="746"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="708"/>
+      <c r="AD9" s="709"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="701"/>
+      <c r="C10" s="702"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13761,7 +13755,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="735"/>
+      <c r="G10" s="736"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13769,33 +13763,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="714"/>
-      <c r="M10" s="703" t="s">
+      <c r="K10" s="715"/>
+      <c r="M10" s="704" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="704"/>
-      <c r="O10" s="704"/>
-      <c r="P10" s="704"/>
-      <c r="Q10" s="704"/>
-      <c r="R10" s="704"/>
-      <c r="S10" s="704"/>
-      <c r="T10" s="704"/>
-      <c r="U10" s="704"/>
-      <c r="V10" s="704"/>
-      <c r="W10" s="704"/>
-      <c r="X10" s="704"/>
-      <c r="Y10" s="704"/>
-      <c r="Z10" s="704"/>
-      <c r="AA10" s="704"/>
-      <c r="AB10" s="704"/>
-      <c r="AC10" s="705"/>
-      <c r="AD10" s="708"/>
+      <c r="N10" s="705"/>
+      <c r="O10" s="705"/>
+      <c r="P10" s="705"/>
+      <c r="Q10" s="705"/>
+      <c r="R10" s="705"/>
+      <c r="S10" s="705"/>
+      <c r="T10" s="705"/>
+      <c r="U10" s="705"/>
+      <c r="V10" s="705"/>
+      <c r="W10" s="705"/>
+      <c r="X10" s="705"/>
+      <c r="Y10" s="705"/>
+      <c r="Z10" s="705"/>
+      <c r="AA10" s="705"/>
+      <c r="AB10" s="705"/>
+      <c r="AC10" s="706"/>
+      <c r="AD10" s="709"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="702"/>
-      <c r="G11" s="735"/>
+      <c r="C11" s="703"/>
+      <c r="G11" s="736"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="714"/>
+      <c r="K11" s="715"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13803,17 +13797,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="724" t="s">
+      <c r="Z11" s="725" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="725"/>
+      <c r="AA11" s="726"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="708"/>
+      <c r="AD11" s="709"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13826,7 +13820,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="735"/>
+      <c r="G12" s="736"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13834,8 +13828,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="714"/>
-      <c r="L12" s="729" t="s">
+      <c r="K12" s="715"/>
+      <c r="L12" s="730" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13850,7 +13844,7 @@
       <c r="Q12" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="S12" s="559" t="s">
+      <c r="S12" s="560" t="s">
         <v>107</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -13866,26 +13860,26 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="718" t="s">
+      <c r="AA12" s="719" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="719"/>
+      <c r="AB12" s="720"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="708"/>
+      <c r="AD12" s="709"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="700"/>
-      <c r="G13" s="735"/>
-      <c r="K13" s="714"/>
-      <c r="L13" s="730"/>
+      <c r="C13" s="701"/>
+      <c r="G13" s="736"/>
+      <c r="K13" s="715"/>
+      <c r="L13" s="731"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="737" t="s">
+      <c r="Q13" s="738" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="633"/>
-      <c r="S13" s="560"/>
+      <c r="R13" s="634"/>
+      <c r="S13" s="561"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
         <v>132</v>
@@ -13893,17 +13887,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="720"/>
-      <c r="AB13" s="721"/>
-      <c r="AD13" s="708"/>
+      <c r="AA13" s="721"/>
+      <c r="AB13" s="722"/>
+      <c r="AD13" s="709"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="702"/>
+      <c r="C14" s="703"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="735"/>
+      <c r="G14" s="736"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13911,8 +13905,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="714"/>
-      <c r="L14" s="730"/>
+      <c r="K14" s="715"/>
+      <c r="L14" s="731"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13922,7 +13916,7 @@
       <c r="R14" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="S14" s="560"/>
+      <c r="S14" s="561"/>
       <c r="T14" s="77" t="s">
         <v>130</v>
       </c>
@@ -13933,9 +13927,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="720"/>
-      <c r="AB14" s="721"/>
-      <c r="AD14" s="708"/>
+      <c r="AA14" s="721"/>
+      <c r="AB14" s="722"/>
+      <c r="AD14" s="709"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13950,20 +13944,20 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="735"/>
+      <c r="G15" s="736"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="714"/>
-      <c r="L15" s="731"/>
-      <c r="Q15" s="737" t="s">
+      <c r="K15" s="715"/>
+      <c r="L15" s="732"/>
+      <c r="Q15" s="738" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="633"/>
-      <c r="S15" s="560"/>
+      <c r="R15" s="634"/>
+      <c r="S15" s="561"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
         <v>44</v>
@@ -13971,14 +13965,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="720"/>
-      <c r="AB15" s="721"/>
-      <c r="AD15" s="708"/>
+      <c r="AA15" s="721"/>
+      <c r="AB15" s="722"/>
+      <c r="AD15" s="709"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="735"/>
-      <c r="K16" s="714"/>
+      <c r="G16" s="736"/>
+      <c r="K16" s="715"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13986,7 +13980,7 @@
       <c r="R16" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="S16" s="560"/>
+      <c r="S16" s="561"/>
       <c r="T16" s="76" t="s">
         <v>129</v>
       </c>
@@ -13997,34 +13991,34 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="720"/>
-      <c r="AB16" s="721"/>
-      <c r="AD16" s="708"/>
+      <c r="AA16" s="721"/>
+      <c r="AB16" s="722"/>
+      <c r="AD16" s="709"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="732" t="s">
+      <c r="F17" s="733" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="735"/>
+      <c r="G17" s="736"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="714"/>
-      <c r="S17" s="560"/>
+      <c r="K17" s="715"/>
+      <c r="S17" s="561"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="720"/>
-      <c r="AB17" s="721"/>
-      <c r="AD17" s="708"/>
+      <c r="AA17" s="721"/>
+      <c r="AB17" s="722"/>
+      <c r="AD17" s="709"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14034,50 +14028,50 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="733"/>
-      <c r="G18" s="735"/>
+      <c r="F18" s="734"/>
+      <c r="G18" s="736"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="714"/>
+      <c r="K18" s="715"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="S18" s="560"/>
+      <c r="S18" s="561"/>
       <c r="U18" s="76" t="s">
         <v>133</v>
       </c>
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="722"/>
-      <c r="AB18" s="723"/>
-      <c r="AD18" s="708"/>
+      <c r="AA18" s="723"/>
+      <c r="AB18" s="724"/>
+      <c r="AD18" s="709"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="736"/>
-      <c r="K19" s="715"/>
+      <c r="G19" s="737"/>
+      <c r="K19" s="716"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="741" t="s">
+      <c r="R19" s="742" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="742"/>
-      <c r="T19" s="743"/>
+      <c r="S19" s="743"/>
+      <c r="T19" s="744"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="709"/>
+      <c r="AD19" s="710"/>
     </row>
   </sheetData>
   <mergeCells count="24">

</xml_diff>

<commit_message>
Boat Halted - France24 F
Boat Halted - France24 F
</commit_message>
<xml_diff>
--- a/System_2.1.7.xlsx
+++ b/System_2.1.7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F124BEAE-6572-46EB-B7D0-86339D417152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95433C41-CAF5-4EBC-B4B0-902E2FE27DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="628">
   <si>
     <t>Zone</t>
   </si>
@@ -1914,6 +1914,15 @@
   </si>
   <si>
     <t>nd tv india</t>
+  </si>
+  <si>
+    <t>rbharat</t>
+  </si>
+  <si>
+    <t>timesnow</t>
+  </si>
+  <si>
+    <t>nd tv 24*7</t>
   </si>
 </sst>
 </file>
@@ -3500,7 +3509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="747">
+  <cellXfs count="758">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4752,9 +4761,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4831,6 +4837,9 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4879,6 +4888,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="27" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4936,43 +4984,139 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5047,140 +5191,62 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5194,63 +5260,6 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="52" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5269,46 +5278,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5386,29 +5374,77 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="48" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5418,10 +5454,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF990033"/>
+      <color rgb="FFFF99CC"/>
       <color rgb="FFFF99FF"/>
-      <color rgb="FFFF99CC"/>
       <color rgb="FFC4B286"/>
-      <color rgb="FF990033"/>
       <color rgb="FFEBF2A6"/>
     </mruColors>
   </colors>
@@ -5701,7 +5737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
@@ -6265,7 +6301,7 @@
       <c r="Q16" s="19" t="s">
         <v>604</v>
       </c>
-      <c r="R16" s="544" t="s">
+      <c r="R16" s="543" t="s">
         <v>42</v>
       </c>
       <c r="S16" s="112">
@@ -6550,7 +6586,7 @@
       <c r="O24" s="500" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="547"/>
+      <c r="P24" s="546"/>
       <c r="S24" s="80"/>
       <c r="T24" s="568"/>
     </row>
@@ -6627,7 +6663,7 @@
       </c>
       <c r="P26" s="321"/>
       <c r="T26" s="568"/>
-      <c r="V26" s="548" t="s">
+      <c r="V26" s="547" t="s">
         <v>618</v>
       </c>
     </row>
@@ -6732,8 +6768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:AK31"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+    <sheetView topLeftCell="N12" workbookViewId="0">
+      <selection activeCell="AB29" sqref="AB29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6800,7 +6836,7 @@
       <c r="P1" s="422" t="s">
         <v>406</v>
       </c>
-      <c r="Q1" s="592" t="s">
+      <c r="Q1" s="573" t="s">
         <v>181</v>
       </c>
       <c r="R1" s="100" t="s">
@@ -6821,10 +6857,10 @@
       <c r="Z1" s="24" t="s">
         <v>584</v>
       </c>
-      <c r="AA1" s="552" t="s">
+      <c r="AA1" s="551" t="s">
         <v>452</v>
       </c>
-      <c r="AB1" s="599" t="s">
+      <c r="AB1" s="580" t="s">
         <v>615</v>
       </c>
       <c r="AC1" s="99" t="s">
@@ -6845,32 +6881,32 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="573">
+      <c r="A2" s="586">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="575" t="s">
+      <c r="B2" s="588" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="587" t="s">
+      <c r="C2" s="600" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="577" t="s">
+      <c r="D2" s="590" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="579" t="s">
+      <c r="E2" s="592" t="s">
         <v>65</v>
       </c>
       <c r="F2" s="196" t="s">
         <v>220</v>
       </c>
-      <c r="G2" s="585" t="s">
+      <c r="G2" s="598" t="s">
         <v>379</v>
       </c>
       <c r="H2" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I2" s="596" t="s">
+      <c r="I2" s="577" t="s">
         <v>103</v>
       </c>
       <c r="J2" s="420" t="s">
@@ -6894,7 +6930,7 @@
       <c r="P2" s="423">
         <v>40</v>
       </c>
-      <c r="Q2" s="593"/>
+      <c r="Q2" s="574"/>
       <c r="R2" s="21">
         <f>R7+R20</f>
         <v>3</v>
@@ -6919,10 +6955,14 @@
         <f>IF((Z2+T2)&gt;0,0,-1)</f>
         <v>0</v>
       </c>
-      <c r="AB2" s="600"/>
+      <c r="AB2" s="581"/>
       <c r="AC2" s="35"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="494"/>
+      <c r="AH2" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="AI2" s="494">
+        <v>1</v>
+      </c>
       <c r="AJ2" s="6" t="s">
         <v>467</v>
       </c>
@@ -6931,14 +6971,14 @@
       </c>
     </row>
     <row r="3" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="574"/>
-      <c r="B3" s="576"/>
-      <c r="C3" s="588"/>
-      <c r="D3" s="578"/>
-      <c r="E3" s="580"/>
-      <c r="G3" s="586"/>
+      <c r="A3" s="587"/>
+      <c r="B3" s="589"/>
+      <c r="C3" s="601"/>
+      <c r="D3" s="591"/>
+      <c r="E3" s="593"/>
+      <c r="G3" s="599"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="597"/>
+      <c r="I3" s="578"/>
       <c r="K3" s="24">
         <v>2</v>
       </c>
@@ -6947,13 +6987,13 @@
       </c>
       <c r="Q3" s="496">
         <f>SUM(X23:X31)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U3" s="6"/>
       <c r="V3" s="495"/>
       <c r="W3" s="6"/>
       <c r="X3" s="495"/>
-      <c r="AB3" s="600"/>
+      <c r="AB3" s="581"/>
       <c r="AC3" s="35"/>
       <c r="AE3" s="100" t="s">
         <v>610</v>
@@ -6963,8 +7003,12 @@
         <f>IF((AE7-SUM(AI2:AI10)&lt;0),AE7-SUM(AK2:AK10),0)</f>
         <v>0</v>
       </c>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="495"/>
+      <c r="AH3" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="AI3" s="495">
+        <v>1</v>
+      </c>
       <c r="AJ3" s="6" t="s">
         <v>252</v>
       </c>
@@ -6977,10 +7021,10 @@
         <v>388</v>
       </c>
       <c r="B4" s="248"/>
-      <c r="C4" s="581" t="s">
+      <c r="C4" s="594" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="597"/>
+      <c r="I4" s="578"/>
       <c r="R4" s="496" t="s">
         <v>610</v>
       </c>
@@ -6992,7 +7036,7 @@
       <c r="V4" s="495"/>
       <c r="W4" s="6"/>
       <c r="X4" s="495"/>
-      <c r="AB4" s="600"/>
+      <c r="AB4" s="581"/>
       <c r="AC4" s="35"/>
       <c r="AE4" s="20"/>
       <c r="AF4" s="100" t="s">
@@ -7002,10 +7046,18 @@
         <f>IF((AF7-SUM(AI2:AI10)&lt;0),AF7-SUM(AK2:AK10),0)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="495"/>
-      <c r="AJ4" s="6"/>
-      <c r="AK4" s="495"/>
+      <c r="AH4" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="AI4" s="495">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="AK4" s="495">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="226" t="s">
@@ -7014,7 +7066,7 @@
       <c r="B5" s="100" t="s">
         <v>364</v>
       </c>
-      <c r="C5" s="582"/>
+      <c r="C5" s="595"/>
       <c r="D5" s="227" t="s">
         <v>103</v>
       </c>
@@ -7030,7 +7082,7 @@
       <c r="H5" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I5" s="597"/>
+      <c r="I5" s="578"/>
       <c r="J5" s="421" t="s">
         <v>273</v>
       </c>
@@ -7057,7 +7109,7 @@
       <c r="V5" s="493"/>
       <c r="W5" s="6"/>
       <c r="X5" s="493"/>
-      <c r="AB5" s="600"/>
+      <c r="AB5" s="581"/>
       <c r="AC5" s="2" t="s">
         <v>613</v>
       </c>
@@ -7078,19 +7130,19 @@
       </c>
     </row>
     <row r="6" spans="1:37" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="570" t="s">
+      <c r="A6" s="583" t="s">
         <v>290</v>
       </c>
       <c r="B6" s="105" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="583"/>
-      <c r="D6" s="584"/>
+      <c r="C6" s="596"/>
+      <c r="D6" s="597"/>
       <c r="E6" s="96">
         <v>1</v>
       </c>
       <c r="G6" s="560"/>
-      <c r="I6" s="597"/>
+      <c r="I6" s="578"/>
       <c r="P6" s="61" t="s">
         <v>613</v>
       </c>
@@ -7102,21 +7154,22 @@
         <f>S7-S12-SUM(V2:V10)</f>
         <v>0</v>
       </c>
-      <c r="AB6" s="600"/>
+      <c r="AB6" s="581"/>
       <c r="AC6" s="35"/>
       <c r="AE6" s="64">
         <f>AE7-SUM(AI1:AI10)+AE11</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="64">
         <f>AF7-SUM(AK2:AK10)+AF11</f>
-        <v>4</v>
-      </c>
-      <c r="AI6" s="20"/>
-      <c r="AK6" s="342"/>
+        <v>1</v>
+      </c>
+      <c r="AI6" s="112"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="757"/>
     </row>
     <row r="7" spans="1:37" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="571"/>
+      <c r="A7" s="584"/>
       <c r="B7" s="100" t="s">
         <v>155</v>
       </c>
@@ -7127,7 +7180,7 @@
         <v>136</v>
       </c>
       <c r="G7" s="560"/>
-      <c r="I7" s="597"/>
+      <c r="I7" s="578"/>
       <c r="M7" s="16" t="s">
         <v>354</v>
       </c>
@@ -7159,7 +7212,7 @@
       <c r="X7" s="494">
         <v>1</v>
       </c>
-      <c r="AB7" s="600"/>
+      <c r="AB7" s="581"/>
       <c r="AC7" s="99" t="s">
         <v>614</v>
       </c>
@@ -7168,11 +7221,11 @@
       </c>
       <c r="AE7" s="24">
         <f>8-AE11</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AF7" s="301">
         <f>8-AF11</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH7" s="6" t="s">
         <v>247</v>
@@ -7184,7 +7237,7 @@
       <c r="AK7" s="494"/>
     </row>
     <row r="8" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="572"/>
+      <c r="A8" s="585"/>
       <c r="B8" s="217" t="s">
         <v>28</v>
       </c>
@@ -7193,14 +7246,14 @@
         <v>3</v>
       </c>
       <c r="G8" s="560"/>
-      <c r="I8" s="597"/>
+      <c r="I8" s="578"/>
       <c r="N8" s="80"/>
       <c r="U8" s="6"/>
       <c r="V8" s="24"/>
       <c r="W8" s="6"/>
       <c r="X8" s="492"/>
-      <c r="AB8" s="600"/>
-      <c r="AC8" s="550"/>
+      <c r="AB8" s="581"/>
+      <c r="AC8" s="549"/>
       <c r="AH8" s="6" t="s">
         <v>622</v>
       </c>
@@ -7229,7 +7282,7 @@
       </c>
       <c r="G9" s="560"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="597"/>
+      <c r="I9" s="578"/>
       <c r="M9" s="19" t="s">
         <v>542</v>
       </c>
@@ -7237,8 +7290,8 @@
       <c r="U9" s="6"/>
       <c r="V9" s="24"/>
       <c r="X9" s="492"/>
-      <c r="AB9" s="600"/>
-      <c r="AC9" s="550"/>
+      <c r="AB9" s="581"/>
+      <c r="AC9" s="549"/>
       <c r="AE9" s="20"/>
       <c r="AF9" s="20"/>
       <c r="AH9" s="6" t="s">
@@ -7247,7 +7300,12 @@
       <c r="AI9" s="24">
         <v>1</v>
       </c>
-      <c r="AK9" s="492"/>
+      <c r="AJ9" s="756" t="s">
+        <v>624</v>
+      </c>
+      <c r="AK9" s="495">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="237" t="s">
@@ -7260,10 +7318,10 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!U8</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="560"/>
-      <c r="I10" s="597"/>
+      <c r="I10" s="578"/>
       <c r="J10" s="24" t="s">
         <v>379</v>
       </c>
@@ -7278,8 +7336,8 @@
       <c r="V10" s="495"/>
       <c r="W10" s="6"/>
       <c r="X10" s="492"/>
-      <c r="AB10" s="600"/>
-      <c r="AC10" s="550"/>
+      <c r="AB10" s="581"/>
+      <c r="AC10" s="549"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AH10" s="6" t="s">
@@ -7288,8 +7346,12 @@
       <c r="AI10" s="495">
         <v>1</v>
       </c>
-      <c r="AJ10" s="6"/>
-      <c r="AK10" s="492"/>
+      <c r="AJ10" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="AK10" s="495">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
@@ -7305,7 +7367,7 @@
         <v>270</v>
       </c>
       <c r="G11" s="560"/>
-      <c r="I11" s="597"/>
+      <c r="I11" s="578"/>
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
@@ -7331,13 +7393,13 @@
       <c r="S11" s="24">
         <v>3</v>
       </c>
-      <c r="U11" s="589" t="s">
+      <c r="U11" s="570" t="s">
         <v>576</v>
       </c>
-      <c r="V11" s="590"/>
-      <c r="W11" s="590"/>
-      <c r="X11" s="591"/>
-      <c r="AB11" s="601"/>
+      <c r="V11" s="571"/>
+      <c r="W11" s="571"/>
+      <c r="X11" s="572"/>
+      <c r="AB11" s="582"/>
       <c r="AC11" s="99" t="s">
         <v>616</v>
       </c>
@@ -7345,18 +7407,18 @@
         <v>44</v>
       </c>
       <c r="AE11" s="24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF11" s="24">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AG11" s="438"/>
-      <c r="AH11" s="589" t="s">
+      <c r="AH11" s="570" t="s">
         <v>576</v>
       </c>
-      <c r="AI11" s="590"/>
-      <c r="AJ11" s="590"/>
-      <c r="AK11" s="591"/>
+      <c r="AI11" s="571"/>
+      <c r="AJ11" s="571"/>
+      <c r="AK11" s="572"/>
     </row>
     <row r="12" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="232" t="s">
@@ -7367,7 +7429,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="560"/>
-      <c r="I12" s="597"/>
+      <c r="I12" s="578"/>
       <c r="J12" s="24" t="s">
         <v>533</v>
       </c>
@@ -7400,7 +7462,7 @@
       </c>
       <c r="D13" s="20"/>
       <c r="G13" s="560"/>
-      <c r="I13" s="597"/>
+      <c r="I13" s="578"/>
       <c r="J13" s="108" t="s">
         <v>566</v>
       </c>
@@ -7419,7 +7481,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="112"/>
       <c r="W13" s="6"/>
-      <c r="Z13" s="551" t="s">
+      <c r="Z13" s="550" t="s">
         <v>260</v>
       </c>
     </row>
@@ -7444,7 +7506,7 @@
       <c r="H14" s="211" t="s">
         <v>220</v>
       </c>
-      <c r="I14" s="597"/>
+      <c r="I14" s="578"/>
       <c r="U14" s="67" t="s">
         <v>81</v>
       </c>
@@ -7455,7 +7517,7 @@
       <c r="X14"/>
       <c r="Z14" s="68">
         <f>SUM(X23:X31)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7471,7 +7533,7 @@
       <c r="H15" s="277">
         <v>0</v>
       </c>
-      <c r="I15" s="597"/>
+      <c r="I15" s="578"/>
       <c r="J15" s="108" t="s">
         <v>154</v>
       </c>
@@ -7502,7 +7564,7 @@
       <c r="D16" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="I16" s="597"/>
+      <c r="I16" s="578"/>
       <c r="K16" s="100" t="s">
         <v>44</v>
       </c>
@@ -7546,7 +7608,7 @@
       <c r="G17" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="I17" s="597"/>
+      <c r="I17" s="578"/>
       <c r="L17" s="2" t="s">
         <v>441</v>
       </c>
@@ -7564,13 +7626,13 @@
     </row>
     <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="16"/>
-      <c r="I18" s="597"/>
+      <c r="I18" s="578"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="O18" s="594" t="s">
+      <c r="O18" s="575" t="s">
         <v>534</v>
       </c>
-      <c r="P18" s="595"/>
+      <c r="P18" s="576"/>
       <c r="Q18" s="127" t="s">
         <v>44</v>
       </c>
@@ -7596,7 +7658,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="597"/>
+      <c r="I19" s="578"/>
       <c r="M19" s="21" t="s">
         <v>440</v>
       </c>
@@ -7628,7 +7690,7 @@
       <c r="G20" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="I20" s="597"/>
+      <c r="I20" s="578"/>
       <c r="K20" s="19" t="s">
         <v>437</v>
       </c>
@@ -7659,7 +7721,7 @@
       <c r="X20" s="493"/>
     </row>
     <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I21" s="597"/>
+      <c r="I21" s="578"/>
       <c r="M21" s="221" t="s">
         <v>420</v>
       </c>
@@ -7689,7 +7751,7 @@
       <c r="G22" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="I22" s="597"/>
+      <c r="I22" s="578"/>
       <c r="P22" s="99" t="s">
         <v>612</v>
       </c>
@@ -7704,10 +7766,10 @@
       <c r="E23" s="289" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="597"/>
+      <c r="I23" s="578"/>
       <c r="Q23" s="24">
         <f>SUM(V23:V31)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U23" s="354"/>
       <c r="V23" s="188">
@@ -7721,9 +7783,9 @@
       </c>
     </row>
     <row r="24" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="597"/>
+      <c r="I24" s="578"/>
       <c r="U24" s="35"/>
-      <c r="V24" s="539">
+      <c r="V24" s="538">
         <v>1</v>
       </c>
       <c r="W24" s="54" t="s">
@@ -7749,7 +7811,7 @@
       <c r="H25" s="196" t="s">
         <v>271</v>
       </c>
-      <c r="I25" s="597"/>
+      <c r="I25" s="578"/>
       <c r="J25" s="421" t="s">
         <v>274</v>
       </c>
@@ -7763,7 +7825,7 @@
         <v>1</v>
       </c>
       <c r="U25" s="35"/>
-      <c r="V25" s="539">
+      <c r="V25" s="538">
         <v>1</v>
       </c>
       <c r="W25" s="54" t="s">
@@ -7794,7 +7856,7 @@
       <c r="H26" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="I26" s="597"/>
+      <c r="I26" s="578"/>
       <c r="K26" s="24">
         <v>15</v>
       </c>
@@ -7818,7 +7880,7 @@
         <v>574</v>
       </c>
       <c r="U26" s="439"/>
-      <c r="V26" s="539">
+      <c r="V26" s="538">
         <v>0</v>
       </c>
       <c r="W26" s="54" t="s">
@@ -7829,7 +7891,7 @@
       </c>
     </row>
     <row r="27" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I27" s="597"/>
+      <c r="I27" s="578"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
       </c>
@@ -7839,7 +7901,7 @@
       <c r="R27" s="112"/>
       <c r="S27" s="112"/>
       <c r="U27" s="35"/>
-      <c r="V27" s="539">
+      <c r="V27" s="538">
         <v>0</v>
       </c>
       <c r="W27" s="54" t="s">
@@ -7856,12 +7918,12 @@
       <c r="E28" s="220">
         <v>2</v>
       </c>
-      <c r="I28" s="597"/>
+      <c r="I28" s="578"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="142"/>
       <c r="U28" s="35"/>
-      <c r="V28" s="539">
+      <c r="V28" s="538">
         <v>1</v>
       </c>
       <c r="W28" s="54" t="s">
@@ -7878,7 +7940,7 @@
       <c r="H29" s="196" t="s">
         <v>272</v>
       </c>
-      <c r="I29" s="598"/>
+      <c r="I29" s="579"/>
       <c r="J29" s="333"/>
       <c r="L29" s="96" t="s">
         <v>278</v>
@@ -7889,10 +7951,10 @@
       <c r="R29" s="491"/>
       <c r="S29" s="112"/>
       <c r="T29" s="80"/>
-      <c r="U29" s="549" t="s">
+      <c r="U29" s="548" t="s">
         <v>575</v>
       </c>
-      <c r="V29" s="539">
+      <c r="V29" s="538">
         <v>1</v>
       </c>
       <c r="W29" s="54" t="s">
@@ -7909,22 +7971,22 @@
       <c r="B30" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="U30" s="549" t="s">
+      <c r="U30" s="548" t="s">
         <v>601</v>
       </c>
-      <c r="V30" s="539">
-        <v>0</v>
+      <c r="V30" s="538">
+        <v>1</v>
       </c>
       <c r="W30" s="54" t="s">
         <v>577</v>
       </c>
       <c r="X30" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U31" s="506"/>
-      <c r="V31" s="536">
+      <c r="V31" s="535">
         <v>0</v>
       </c>
       <c r="W31" s="54" t="s">
@@ -7936,12 +7998,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AH11:AK11"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="U11:X11"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="I2:I29"/>
-    <mergeCell ref="AB1:AB11"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="G5:G14"/>
@@ -7954,6 +8010,12 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="AH11:AK11"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="U11:X11"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="I2:I29"/>
+    <mergeCell ref="AB1:AB11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7963,7 +8025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -8029,7 +8091,7 @@
       <c r="H1" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="I1" s="585" t="s">
+      <c r="I1" s="598" t="s">
         <v>376</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -8090,7 +8152,7 @@
         <v>513</v>
       </c>
       <c r="AM1" s="426"/>
-      <c r="AN1" s="626"/>
+      <c r="AN1" s="629"/>
       <c r="AO1" s="350" t="s">
         <v>484</v>
       </c>
@@ -8099,23 +8161,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="608">
+      <c r="A2" s="653">
         <f ca="1">TODAY()</f>
         <v>45282</v>
       </c>
-      <c r="B2" s="610" t="s">
+      <c r="B2" s="655" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="587" t="s">
+      <c r="C2" s="600" t="s">
         <v>364</v>
       </c>
-      <c r="D2" s="612" t="s">
+      <c r="D2" s="657" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="656" t="s">
+      <c r="E2" s="602" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="631" t="s">
+      <c r="F2" s="610" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="417" t="s">
@@ -8124,31 +8186,31 @@
       <c r="H2" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="586"/>
+      <c r="I2" s="599"/>
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="658" t="s">
+      <c r="K2" s="604" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="659"/>
-      <c r="M2" s="631" t="s">
+      <c r="L2" s="605"/>
+      <c r="M2" s="610" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="635" t="s">
+      <c r="O2" s="636" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="Q2" s="587" t="s">
+      <c r="Q2" s="600" t="s">
         <v>144</v>
       </c>
       <c r="R2" s="559"/>
-      <c r="S2" s="648" t="s">
+      <c r="S2" s="623" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -8181,15 +8243,15 @@
         <v>478</v>
       </c>
       <c r="AM2" s="452"/>
-      <c r="AN2" s="627"/>
+      <c r="AN2" s="630"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="609"/>
-      <c r="B3" s="611"/>
-      <c r="C3" s="588"/>
-      <c r="D3" s="613"/>
-      <c r="E3" s="657"/>
-      <c r="F3" s="632"/>
+      <c r="A3" s="654"/>
+      <c r="B3" s="656"/>
+      <c r="C3" s="601"/>
+      <c r="D3" s="658"/>
+      <c r="E3" s="603"/>
+      <c r="F3" s="611"/>
       <c r="G3" s="418" t="s">
         <v>28</v>
       </c>
@@ -8208,17 +8270,17 @@
       <c r="L3" s="206" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="632"/>
+      <c r="M3" s="611"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="636"/>
+      <c r="O3" s="637"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="Q3" s="588"/>
+      <c r="Q3" s="601"/>
       <c r="R3" s="561"/>
-      <c r="S3" s="649"/>
+      <c r="S3" s="625"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -8235,7 +8297,7 @@
       <c r="AC3" s="100" t="s">
         <v>495</v>
       </c>
-      <c r="AD3" s="647" t="s">
+      <c r="AD3" s="620" t="s">
         <v>470</v>
       </c>
       <c r="AE3" s="262"/>
@@ -8247,16 +8309,16 @@
       <c r="AK3" s="262"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="452"/>
-      <c r="AN3" s="627"/>
+      <c r="AN3" s="630"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="243" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="624" t="s">
+      <c r="B4" s="669" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="587" t="s">
+      <c r="C4" s="600" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="359" t="s">
@@ -8265,7 +8327,7 @@
       <c r="E4" s="396">
         <v>2</v>
       </c>
-      <c r="F4" s="632"/>
+      <c r="F4" s="611"/>
       <c r="G4" s="400" t="s">
         <v>203</v>
       </c>
@@ -8282,11 +8344,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="209"/>
-      <c r="M4" s="632"/>
+      <c r="M4" s="611"/>
       <c r="N4" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="636"/>
+      <c r="O4" s="637"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -8313,7 +8375,7 @@
       <c r="AA4" s="313"/>
       <c r="AB4" s="214"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="647"/>
+      <c r="AD4" s="620"/>
       <c r="AE4" s="262"/>
       <c r="AF4" s="262"/>
       <c r="AG4" s="16"/>
@@ -8323,37 +8385,37 @@
       <c r="AK4" s="262"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="452"/>
-      <c r="AN4" s="627"/>
+      <c r="AN4" s="630"/>
       <c r="AO4" s="350" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="585" t="s">
+      <c r="A5" s="598" t="s">
         <v>432</v>
       </c>
-      <c r="B5" s="625"/>
-      <c r="C5" s="588"/>
+      <c r="B5" s="670"/>
+      <c r="C5" s="601"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
       </c>
       <c r="E5" s="397">
         <v>1</v>
       </c>
-      <c r="F5" s="632"/>
-      <c r="G5" s="616" t="s">
+      <c r="F5" s="611"/>
+      <c r="G5" s="661" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="616"/>
-      <c r="I5" s="616"/>
-      <c r="J5" s="616"/>
-      <c r="K5" s="616"/>
-      <c r="L5" s="617"/>
-      <c r="M5" s="632"/>
+      <c r="H5" s="661"/>
+      <c r="I5" s="661"/>
+      <c r="J5" s="661"/>
+      <c r="K5" s="661"/>
+      <c r="L5" s="662"/>
+      <c r="M5" s="611"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="636"/>
+      <c r="O5" s="637"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -8384,24 +8446,24 @@
       <c r="AK5" s="262"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="452"/>
-      <c r="AN5" s="627"/>
+      <c r="AN5" s="630"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="586"/>
-      <c r="B6" s="622" t="s">
+      <c r="A6" s="599"/>
+      <c r="B6" s="667" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="583"/>
-      <c r="D6" s="584"/>
-      <c r="F6" s="632"/>
-      <c r="G6" s="618"/>
-      <c r="H6" s="618"/>
-      <c r="I6" s="618"/>
-      <c r="J6" s="618"/>
-      <c r="K6" s="618"/>
-      <c r="L6" s="619"/>
-      <c r="M6" s="632"/>
-      <c r="O6" s="636"/>
+      <c r="C6" s="596"/>
+      <c r="D6" s="597"/>
+      <c r="F6" s="611"/>
+      <c r="G6" s="663"/>
+      <c r="H6" s="663"/>
+      <c r="I6" s="663"/>
+      <c r="J6" s="663"/>
+      <c r="K6" s="663"/>
+      <c r="L6" s="664"/>
+      <c r="M6" s="611"/>
+      <c r="O6" s="637"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -8425,16 +8487,16 @@
       <c r="AF6" s="262"/>
       <c r="AG6" s="262"/>
       <c r="AH6" s="262"/>
-      <c r="AI6" s="641"/>
+      <c r="AI6" s="619"/>
       <c r="AJ6" s="465" t="s">
         <v>473</v>
       </c>
-      <c r="AK6" s="641" t="s">
+      <c r="AK6" s="619" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="262"/>
       <c r="AM6" s="452"/>
-      <c r="AN6" s="627"/>
+      <c r="AN6" s="630"/>
       <c r="AO6" s="350" t="s">
         <v>485</v>
       </c>
@@ -8443,7 +8505,7 @@
       <c r="A7" s="237" t="s">
         <v>591</v>
       </c>
-      <c r="B7" s="623"/>
+      <c r="B7" s="668"/>
       <c r="C7" s="207" t="s">
         <v>381</v>
       </c>
@@ -8453,7 +8515,7 @@
       <c r="E7" s="271">
         <v>3</v>
       </c>
-      <c r="F7" s="632"/>
+      <c r="F7" s="611"/>
       <c r="G7" s="419">
         <v>0</v>
       </c>
@@ -8472,8 +8534,8 @@
       <c r="L7" s="217">
         <v>0</v>
       </c>
-      <c r="M7" s="632"/>
-      <c r="O7" s="636"/>
+      <c r="M7" s="611"/>
+      <c r="O7" s="637"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -8497,18 +8559,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="262"/>
       <c r="AF7" s="262"/>
-      <c r="AG7" s="647" t="s">
+      <c r="AG7" s="620" t="s">
         <v>469</v>
       </c>
       <c r="AH7" s="262"/>
-      <c r="AI7" s="641"/>
+      <c r="AI7" s="619"/>
       <c r="AJ7" s="262"/>
-      <c r="AK7" s="641"/>
+      <c r="AK7" s="619"/>
       <c r="AL7" s="80" t="s">
         <v>511</v>
       </c>
       <c r="AM7" s="452"/>
-      <c r="AN7" s="627"/>
+      <c r="AN7" s="630"/>
       <c r="AP7" s="76" t="s">
         <v>486</v>
       </c>
@@ -8525,27 +8587,27 @@
         <f>SUM(G7:N9)</f>
         <v>15</v>
       </c>
-      <c r="F8" s="632"/>
-      <c r="G8" s="617">
-        <v>0</v>
-      </c>
-      <c r="H8" s="614" t="s">
+      <c r="F8" s="611"/>
+      <c r="G8" s="662">
+        <v>0</v>
+      </c>
+      <c r="H8" s="659" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="559">
         <v>0</v>
       </c>
-      <c r="J8" s="614" t="s">
+      <c r="J8" s="659" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="620"/>
-      <c r="L8" s="650"/>
-      <c r="M8" s="633"/>
-      <c r="N8" s="653">
+      <c r="K8" s="665"/>
+      <c r="L8" s="621"/>
+      <c r="M8" s="634"/>
+      <c r="N8" s="626">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="636"/>
+      <c r="O8" s="637"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -8563,14 +8625,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="262"/>
       <c r="AF8" s="262"/>
-      <c r="AG8" s="647"/>
+      <c r="AG8" s="620"/>
       <c r="AH8" s="262"/>
-      <c r="AI8" s="641"/>
+      <c r="AI8" s="619"/>
       <c r="AJ8" s="262"/>
       <c r="AK8" s="262"/>
       <c r="AL8" s="262"/>
       <c r="AM8" s="452"/>
-      <c r="AN8" s="627"/>
+      <c r="AN8" s="630"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="237" t="s">
@@ -8585,17 +8647,17 @@
       <c r="D9" s="360" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="632"/>
-      <c r="G9" s="619"/>
-      <c r="H9" s="615"/>
+      <c r="F9" s="611"/>
+      <c r="G9" s="664"/>
+      <c r="H9" s="660"/>
       <c r="I9" s="561"/>
-      <c r="J9" s="615"/>
-      <c r="K9" s="621"/>
-      <c r="L9" s="651"/>
-      <c r="M9" s="634"/>
-      <c r="N9" s="654"/>
-      <c r="O9" s="637"/>
-      <c r="S9" s="648" t="s">
+      <c r="J9" s="660"/>
+      <c r="K9" s="666"/>
+      <c r="L9" s="622"/>
+      <c r="M9" s="635"/>
+      <c r="N9" s="627"/>
+      <c r="O9" s="638"/>
+      <c r="S9" s="623" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -8617,16 +8679,16 @@
       </c>
       <c r="AE9" s="262"/>
       <c r="AF9" s="262"/>
-      <c r="AG9" s="647"/>
+      <c r="AG9" s="620"/>
       <c r="AH9" s="262"/>
-      <c r="AI9" s="641"/>
+      <c r="AI9" s="619"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="641" t="s">
+      <c r="AK9" s="619" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="262"/>
       <c r="AM9" s="452"/>
-      <c r="AN9" s="627"/>
+      <c r="AN9" s="630"/>
       <c r="AP9" s="2" t="s">
         <v>523</v>
       </c>
@@ -8641,22 +8703,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="242">
         <f>Boat!U8</f>
-        <v>37</v>
-      </c>
-      <c r="F10" s="632"/>
+        <v>38</v>
+      </c>
+      <c r="F10" s="611"/>
       <c r="N10" s="442" t="s">
         <v>405</v>
       </c>
-      <c r="O10" s="665" t="s">
+      <c r="O10" s="613" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="638" t="s">
+      <c r="P10" s="639" t="s">
         <v>409</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="652"/>
+      <c r="S10" s="624"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -8686,16 +8748,16 @@
       <c r="AF10" s="243" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="647"/>
+      <c r="AG10" s="620"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="641"/>
+      <c r="AI10" s="619"/>
       <c r="AJ10" s="262"/>
-      <c r="AK10" s="641"/>
+      <c r="AK10" s="619"/>
       <c r="AL10" s="262"/>
       <c r="AM10" s="466" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="627"/>
+      <c r="AN10" s="630"/>
       <c r="AO10" s="209" t="s">
         <v>95</v>
       </c>
@@ -8713,18 +8775,18 @@
       <c r="D11" s="174" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="632"/>
+      <c r="F11" s="611"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="666"/>
-      <c r="P11" s="639"/>
+      <c r="O11" s="614"/>
+      <c r="P11" s="640"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="652"/>
+      <c r="S11" s="624"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -8748,14 +8810,14 @@
       <c r="AF11" s="262" t="s">
         <v>491</v>
       </c>
-      <c r="AG11" s="647"/>
+      <c r="AG11" s="620"/>
       <c r="AH11" s="262"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="262"/>
       <c r="AK11" s="262"/>
       <c r="AL11" s="262"/>
       <c r="AM11" s="452"/>
-      <c r="AN11" s="627"/>
+      <c r="AN11" s="630"/>
       <c r="AP11" s="76" t="s">
         <v>499</v>
       </c>
@@ -8774,7 +8836,7 @@
       <c r="E12" s="229">
         <v>3</v>
       </c>
-      <c r="F12" s="632"/>
+      <c r="F12" s="611"/>
       <c r="G12" s="349" t="s">
         <v>409</v>
       </c>
@@ -8783,16 +8845,16 @@
       </c>
       <c r="I12" s="566"/>
       <c r="J12" s="566"/>
-      <c r="K12" s="670"/>
+      <c r="K12" s="618"/>
       <c r="L12" s="208"/>
       <c r="M12" s="208"/>
       <c r="N12" s="208"/>
-      <c r="O12" s="666"/>
-      <c r="P12" s="639"/>
+      <c r="O12" s="614"/>
+      <c r="P12" s="640"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="649"/>
+      <c r="S12" s="625"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -8813,16 +8875,16 @@
       <c r="AC12" s="100" t="s">
         <v>496</v>
       </c>
-      <c r="AD12" s="655" t="s">
+      <c r="AD12" s="628" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="465" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="647" t="s">
+      <c r="AF12" s="620" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="647"/>
+      <c r="AG12" s="620"/>
       <c r="AH12" s="243" t="s">
         <v>264</v>
       </c>
@@ -8835,7 +8897,7 @@
       <c r="AM12" s="642" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="627"/>
+      <c r="AN12" s="630"/>
       <c r="AO12" s="350" t="s">
         <v>97</v>
       </c>
@@ -8847,17 +8909,17 @@
       <c r="E13" s="472">
         <v>-3</v>
       </c>
-      <c r="F13" s="632"/>
+      <c r="F13" s="611"/>
       <c r="G13" s="566" t="s">
         <v>445</v>
       </c>
       <c r="H13" s="566"/>
       <c r="I13" s="566"/>
-      <c r="J13" s="670"/>
+      <c r="J13" s="618"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="666"/>
-      <c r="P13" s="640"/>
+      <c r="O13" s="614"/>
+      <c r="P13" s="641"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8878,8 +8940,8 @@
         <v>515</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="655"/>
-      <c r="AF13" s="647"/>
+      <c r="AD13" s="628"/>
+      <c r="AF13" s="620"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="243" t="s">
         <v>314</v>
@@ -8891,7 +8953,7 @@
       <c r="AK13" s="262"/>
       <c r="AL13" s="262"/>
       <c r="AM13" s="642"/>
-      <c r="AN13" s="627"/>
+      <c r="AN13" s="630"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="474"/>
@@ -8899,18 +8961,18 @@
       <c r="C14" s="483"/>
       <c r="D14" s="476"/>
       <c r="E14" s="477"/>
-      <c r="F14" s="632"/>
+      <c r="F14" s="611"/>
       <c r="G14" s="566" t="s">
         <v>444</v>
       </c>
       <c r="H14" s="566"/>
       <c r="I14" s="566"/>
-      <c r="J14" s="670"/>
+      <c r="J14" s="618"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="666"/>
+      <c r="O14" s="614"/>
       <c r="Q14" s="61" t="s">
         <v>550</v>
       </c>
@@ -8931,9 +8993,9 @@
       <c r="AA14" s="313"/>
       <c r="AB14" s="214"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="655"/>
+      <c r="AD14" s="628"/>
       <c r="AE14" s="262"/>
-      <c r="AF14" s="647"/>
+      <c r="AF14" s="620"/>
       <c r="AG14" s="262"/>
       <c r="AH14" s="262"/>
       <c r="AI14" s="70"/>
@@ -8941,7 +9003,7 @@
       <c r="AK14" s="262"/>
       <c r="AL14" s="262"/>
       <c r="AM14" s="642"/>
-      <c r="AN14" s="627"/>
+      <c r="AN14" s="630"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="473" t="s">
@@ -8950,8 +9012,8 @@
       <c r="C15" s="559" t="s">
         <v>380</v>
       </c>
-      <c r="F15" s="632"/>
-      <c r="O15" s="666"/>
+      <c r="F15" s="611"/>
+      <c r="O15" s="614"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8973,8 +9035,8 @@
       <c r="AC15" s="76" t="s">
         <v>494</v>
       </c>
-      <c r="AD15" s="655"/>
-      <c r="AF15" s="647"/>
+      <c r="AD15" s="628"/>
+      <c r="AF15" s="620"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="243" t="s">
         <v>463</v>
@@ -8988,7 +9050,7 @@
       <c r="AK15" s="262"/>
       <c r="AL15" s="262"/>
       <c r="AM15" s="642"/>
-      <c r="AN15" s="627"/>
+      <c r="AN15" s="630"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -9010,13 +9072,13 @@
       <c r="E16" s="229">
         <v>1</v>
       </c>
-      <c r="F16" s="632"/>
+      <c r="F16" s="611"/>
       <c r="G16" s="349" t="s">
         <v>503</v>
       </c>
       <c r="I16" s="494"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="666"/>
+      <c r="O16" s="614"/>
       <c r="R16" s="459" t="s">
         <v>185</v>
       </c>
@@ -9048,18 +9110,18 @@
       <c r="AM16" s="452" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="627"/>
+      <c r="AN16" s="630"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="632"/>
+      <c r="F17" s="611"/>
       <c r="I17" s="495"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="666"/>
+      <c r="O17" s="614"/>
       <c r="Q17" s="21" t="s">
         <v>548</v>
       </c>
@@ -9104,7 +9166,7 @@
       <c r="AK17" s="262"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="452"/>
-      <c r="AN17" s="627"/>
+      <c r="AN17" s="630"/>
       <c r="AO17" s="209" t="s">
         <v>512</v>
       </c>
@@ -9128,21 +9190,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="632"/>
+      <c r="F18" s="611"/>
       <c r="G18" s="349" t="s">
         <v>545</v>
       </c>
       <c r="I18" s="24"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="666"/>
+      <c r="O18" s="614"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="660" t="s">
+      <c r="R18" s="606" t="s">
         <v>553</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="605" t="s">
+      <c r="U18" s="650" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -9163,7 +9225,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="262"/>
-      <c r="AF18" s="641" t="s">
+      <c r="AF18" s="619" t="s">
         <v>490</v>
       </c>
       <c r="AG18" s="262"/>
@@ -9175,20 +9237,20 @@
       <c r="AK18" s="262"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="452"/>
-      <c r="AN18" s="627"/>
+      <c r="AN18" s="630"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="632"/>
+      <c r="F19" s="611"/>
       <c r="I19" s="224"/>
-      <c r="O19" s="666"/>
-      <c r="R19" s="661"/>
+      <c r="O19" s="614"/>
+      <c r="R19" s="607"/>
       <c r="S19" s="30" t="s">
         <v>551</v>
       </c>
-      <c r="U19" s="606"/>
+      <c r="U19" s="651"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="455" t="s">
@@ -9203,7 +9265,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="262"/>
-      <c r="AF19" s="641"/>
+      <c r="AF19" s="619"/>
       <c r="AG19" s="262"/>
       <c r="AH19" s="262"/>
       <c r="AI19" s="70"/>
@@ -9213,7 +9275,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="452"/>
-      <c r="AN19" s="627"/>
+      <c r="AN19" s="630"/>
       <c r="AP19" s="76" t="s">
         <v>483</v>
       </c>
@@ -9234,19 +9296,19 @@
       <c r="E20" s="461">
         <v>-1</v>
       </c>
-      <c r="F20" s="632"/>
+      <c r="F20" s="611"/>
       <c r="G20" s="349" t="s">
         <v>506</v>
       </c>
       <c r="I20" s="224"/>
-      <c r="O20" s="666"/>
-      <c r="Q20" s="668" t="s">
+      <c r="O20" s="614"/>
+      <c r="Q20" s="616" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="428" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="607"/>
+      <c r="U20" s="652"/>
       <c r="W20" s="429"/>
       <c r="X20" s="456" t="s">
         <v>175</v>
@@ -9276,7 +9338,7 @@
       <c r="AM20" s="400" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="627"/>
+      <c r="AN20" s="630"/>
       <c r="AO20" s="350" t="s">
         <v>475</v>
       </c>
@@ -9297,13 +9359,13 @@
       <c r="E21" s="271">
         <v>0</v>
       </c>
-      <c r="F21" s="632"/>
+      <c r="F21" s="611"/>
       <c r="I21" s="224"/>
-      <c r="O21" s="666"/>
-      <c r="Q21" s="669"/>
+      <c r="O21" s="614"/>
+      <c r="Q21" s="617"/>
       <c r="T21" s="446"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="602"/>
+      <c r="V21" s="647"/>
       <c r="W21" s="450" t="s">
         <v>176</v>
       </c>
@@ -9341,15 +9403,15 @@
       <c r="AM21" s="452" t="s">
         <v>562</v>
       </c>
-      <c r="AN21" s="627"/>
+      <c r="AN21" s="630"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="632"/>
+      <c r="F22" s="611"/>
       <c r="G22" s="349" t="s">
         <v>504</v>
       </c>
       <c r="I22" s="224"/>
-      <c r="O22" s="666"/>
+      <c r="O22" s="614"/>
       <c r="R22" s="458" t="s">
         <v>44</v>
       </c>
@@ -9357,7 +9419,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="603"/>
+      <c r="V22" s="648"/>
       <c r="W22" s="450" t="s">
         <v>176</v>
       </c>
@@ -9375,7 +9437,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="641" t="s">
+      <c r="AJ22" s="619" t="s">
         <v>487</v>
       </c>
       <c r="AK22" s="262"/>
@@ -9383,7 +9445,7 @@
         <v>493</v>
       </c>
       <c r="AM22" s="306"/>
-      <c r="AN22" s="627"/>
+      <c r="AN22" s="630"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="236" t="s">
@@ -9401,17 +9463,17 @@
       <c r="E23" s="230">
         <v>1</v>
       </c>
-      <c r="F23" s="632"/>
+      <c r="F23" s="611"/>
       <c r="I23" s="224"/>
-      <c r="O23" s="666"/>
-      <c r="Q23" s="668" t="s">
+      <c r="O23" s="614"/>
+      <c r="Q23" s="616" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="444" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="603"/>
+      <c r="V23" s="648"/>
       <c r="W23" s="148"/>
       <c r="X23" s="453" t="s">
         <v>189</v>
@@ -9427,13 +9489,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="641"/>
+      <c r="AJ23" s="619"/>
       <c r="AK23" s="262"/>
       <c r="AL23" s="80" t="s">
         <v>522</v>
       </c>
       <c r="AM23" s="306"/>
-      <c r="AN23" s="627"/>
+      <c r="AN23" s="630"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="464" t="s">
@@ -9451,18 +9513,18 @@
       <c r="E24" s="460">
         <v>1</v>
       </c>
-      <c r="F24" s="632"/>
+      <c r="F24" s="611"/>
       <c r="G24" s="61" t="s">
         <v>505</v>
       </c>
       <c r="I24" s="224"/>
-      <c r="O24" s="666"/>
-      <c r="Q24" s="669"/>
+      <c r="O24" s="614"/>
+      <c r="Q24" s="617"/>
       <c r="T24" s="17"/>
       <c r="U24" s="232" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="603"/>
+      <c r="V24" s="648"/>
       <c r="W24" s="148"/>
       <c r="X24" s="453" t="s">
         <v>186</v>
@@ -9486,12 +9548,12 @@
         <v>478</v>
       </c>
       <c r="AM24" s="306"/>
-      <c r="AN24" s="627"/>
+      <c r="AN24" s="630"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="632"/>
+      <c r="F25" s="611"/>
       <c r="I25" s="224"/>
-      <c r="O25" s="666"/>
+      <c r="O25" s="614"/>
       <c r="P25" s="209" t="s">
         <v>285</v>
       </c>
@@ -9504,7 +9566,7 @@
       <c r="U25" s="424" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="604"/>
+      <c r="V25" s="649"/>
       <c r="W25" s="148"/>
       <c r="X25" s="453" t="s">
         <v>190</v>
@@ -9526,7 +9588,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="306"/>
-      <c r="AN25" s="627"/>
+      <c r="AN25" s="630"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="236" t="s">
@@ -9544,17 +9606,17 @@
       <c r="E26" s="398">
         <v>1</v>
       </c>
-      <c r="F26" s="632"/>
+      <c r="F26" s="611"/>
       <c r="G26" s="349" t="s">
         <v>502</v>
       </c>
       <c r="I26" s="224"/>
-      <c r="O26" s="666"/>
-      <c r="P26" s="629" t="s">
+      <c r="O26" s="614"/>
+      <c r="P26" s="632" t="s">
         <v>543</v>
       </c>
-      <c r="Q26" s="630"/>
-      <c r="R26" s="662" t="s">
+      <c r="Q26" s="633"/>
+      <c r="R26" s="608" t="s">
         <v>552</v>
       </c>
       <c r="T26" s="182"/>
@@ -9593,7 +9655,7 @@
       <c r="AM26" s="466" t="s">
         <v>471</v>
       </c>
-      <c r="AN26" s="627"/>
+      <c r="AN26" s="630"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -9605,13 +9667,13 @@
       <c r="E27" s="271" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="664"/>
+      <c r="F27" s="612"/>
       <c r="G27" s="61" t="s">
         <v>561</v>
       </c>
       <c r="I27" s="225"/>
-      <c r="O27" s="667"/>
-      <c r="R27" s="663"/>
+      <c r="O27" s="615"/>
+      <c r="R27" s="609"/>
       <c r="S27" s="445" t="s">
         <v>54</v>
       </c>
@@ -9641,32 +9703,26 @@
       <c r="AM27" s="400" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="628"/>
+      <c r="AN27" s="631"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -9683,22 +9739,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9708,8 +9770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+    <sheetView tabSelected="1" topLeftCell="M3" workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9804,10 +9866,10 @@
       <c r="S1" s="142"/>
       <c r="T1" s="142"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="678" t="s">
+      <c r="V1" s="674" t="s">
         <v>456</v>
       </c>
-      <c r="W1" s="679"/>
+      <c r="W1" s="675"/>
       <c r="X1" s="312">
         <f>68-(U8+W3+V3+S3)</f>
         <v>0</v>
@@ -9823,28 +9885,28 @@
       <c r="AB1" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="680" t="s">
+      <c r="AC1" s="676" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="681"/>
-      <c r="AE1" s="682"/>
-      <c r="AF1" s="683" t="s">
+      <c r="AD1" s="677"/>
+      <c r="AE1" s="678"/>
+      <c r="AF1" s="679" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="684"/>
-      <c r="AH1" s="685"/>
-      <c r="AI1" s="675" t="s">
+      <c r="AG1" s="680"/>
+      <c r="AH1" s="681"/>
+      <c r="AI1" s="671" t="s">
         <v>459</v>
       </c>
-      <c r="AJ1" s="676"/>
-      <c r="AK1" s="677"/>
+      <c r="AJ1" s="672"/>
+      <c r="AK1" s="673"/>
       <c r="AN1" s="142"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H2" s="537">
+      <c r="H2" s="536">
         <f>SUM(H4:H37)</f>
         <v>-16</v>
       </c>
@@ -9854,19 +9916,19 @@
       <c r="K2" s="327">
         <v>-3</v>
       </c>
-      <c r="L2" s="686">
+      <c r="L2" s="682">
         <f>SUM(L5:L30)</f>
         <v>2</v>
       </c>
-      <c r="M2" s="688">
+      <c r="M2" s="684">
         <f>SUM(M4:M29)</f>
-        <v>12</v>
-      </c>
-      <c r="N2" s="690">
+        <v>11</v>
+      </c>
+      <c r="N2" s="686">
         <f>SUM(N4:N29)</f>
-        <v>11</v>
-      </c>
-      <c r="O2" s="653">
+        <v>9</v>
+      </c>
+      <c r="O2" s="626">
         <f>SUM(M30:M37)* (-1)</f>
         <v>-3</v>
       </c>
@@ -9885,7 +9947,7 @@
       <c r="T2" s="508" t="s">
         <v>221</v>
       </c>
-      <c r="U2" s="692" t="s">
+      <c r="U2" s="688" t="s">
         <v>239</v>
       </c>
       <c r="V2" s="509" t="s">
@@ -9954,10 +10016,10 @@
         <f>T3+V3+W3+S3</f>
         <v>68</v>
       </c>
-      <c r="L3" s="687"/>
-      <c r="M3" s="689"/>
-      <c r="N3" s="691"/>
-      <c r="O3" s="654"/>
+      <c r="L3" s="683"/>
+      <c r="M3" s="685"/>
+      <c r="N3" s="687"/>
+      <c r="O3" s="627"/>
       <c r="P3" s="176">
         <f>(L2+M2)-W3</f>
         <v>0</v>
@@ -9971,16 +10033,16 @@
       </c>
       <c r="T3" s="511">
         <f>SUM(T4:T29)</f>
-        <v>37</v>
-      </c>
-      <c r="U3" s="693"/>
+        <v>38</v>
+      </c>
+      <c r="U3" s="689"/>
       <c r="V3" s="512">
         <f t="shared" ref="V3:AA3" si="0">SUM(V4:V29)</f>
         <v>5</v>
       </c>
       <c r="W3" s="512">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9988,23 +10050,23 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -10016,7 +10078,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AG3" s="386">
         <f t="shared" si="1"/>
@@ -10028,15 +10090,15 @@
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AJ3" s="317">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AK3" s="318">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AN3" s="142"/>
     </row>
@@ -10072,7 +10134,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="O4" s="672" t="s">
+      <c r="O4" s="691" t="s">
         <v>200</v>
       </c>
       <c r="P4" s="20"/>
@@ -10133,7 +10195,7 @@
         <f>IF((AI4-AJ4)&gt;AJ4,(AI4-AJ4),AJ4)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="534" t="s">
+      <c r="AL4" s="533" t="s">
         <v>204</v>
       </c>
       <c r="AM4" s="188"/>
@@ -10151,7 +10213,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="O5" s="673"/>
+      <c r="O5" s="692"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="2" t="s">
         <v>347</v>
@@ -10209,7 +10271,7 @@
         <v>0</v>
       </c>
       <c r="AL5" s="6"/>
-      <c r="AM5" s="538"/>
+      <c r="AM5" s="537"/>
       <c r="AN5" s="142"/>
     </row>
     <row r="6" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10238,26 +10300,26 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="O6" s="673"/>
+      <c r="O6" s="692"/>
       <c r="P6" s="19" t="s">
         <v>342</v>
       </c>
       <c r="R6" s="321" t="s">
         <v>231</v>
       </c>
-      <c r="S6" s="522">
+      <c r="S6" s="751">
         <v>2</v>
       </c>
-      <c r="T6" s="523">
+      <c r="T6" s="746">
         <v>2</v>
       </c>
-      <c r="U6" s="520">
+      <c r="U6" s="747">
         <v>-2</v>
       </c>
-      <c r="V6" s="524">
+      <c r="V6" s="750">
         <v>2</v>
       </c>
-      <c r="W6" s="517">
+      <c r="W6" s="748">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10303,7 +10365,7 @@
         <v>0</v>
       </c>
       <c r="AL6" s="6"/>
-      <c r="AM6" s="539" t="s">
+      <c r="AM6" s="538" t="s">
         <v>578</v>
       </c>
       <c r="AN6" s="142" t="s">
@@ -10332,7 +10394,7 @@
         <f t="shared" ref="N7:N37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="673"/>
+      <c r="O7" s="692"/>
       <c r="P7" s="20"/>
       <c r="Q7" s="2" t="s">
         <v>342</v>
@@ -10340,19 +10402,19 @@
       <c r="R7" s="321" t="s">
         <v>245</v>
       </c>
-      <c r="S7" s="525">
-        <v>1</v>
-      </c>
-      <c r="T7" s="526">
+      <c r="S7" s="551">
+        <v>1</v>
+      </c>
+      <c r="T7" s="755">
         <v>2</v>
       </c>
-      <c r="U7" s="527">
+      <c r="U7" s="749">
         <v>-2</v>
       </c>
-      <c r="V7" s="524">
+      <c r="V7" s="752">
         <v>2</v>
       </c>
-      <c r="W7" s="517">
+      <c r="W7" s="748">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -10402,7 +10464,7 @@
       <c r="AL7" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="AM7" s="539"/>
+      <c r="AM7" s="538"/>
       <c r="AN7" s="262"/>
     </row>
     <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10440,7 +10502,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O8" s="673"/>
+      <c r="O8" s="692"/>
       <c r="P8" s="21" t="s">
         <v>238</v>
       </c>
@@ -10450,15 +10512,15 @@
       <c r="R8" s="322" t="s">
         <v>202</v>
       </c>
-      <c r="S8" s="528">
-        <v>0</v>
-      </c>
-      <c r="T8" s="26">
-        <v>1</v>
-      </c>
-      <c r="U8" s="29">
+      <c r="S8" s="527">
+        <v>0</v>
+      </c>
+      <c r="T8" s="753">
+        <v>1</v>
+      </c>
+      <c r="U8" s="754">
         <f>T3</f>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="V8" s="524">
         <v>0</v>
@@ -10509,7 +10571,7 @@
         <v>0</v>
       </c>
       <c r="AL8" s="6"/>
-      <c r="AM8" s="539"/>
+      <c r="AM8" s="538"/>
       <c r="AN8" s="262"/>
     </row>
     <row r="9" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10524,21 +10586,21 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O9" s="673"/>
+      <c r="O9" s="692"/>
       <c r="P9" s="21" t="s">
         <v>342</v>
       </c>
       <c r="R9" s="322" t="s">
         <v>264</v>
       </c>
-      <c r="S9" s="529"/>
-      <c r="T9" s="530">
+      <c r="S9" s="528"/>
+      <c r="T9" s="529">
         <v>2</v>
       </c>
       <c r="U9" s="515">
         <v>-2</v>
       </c>
-      <c r="V9" s="531"/>
+      <c r="V9" s="530"/>
       <c r="W9" s="517">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -10587,7 +10649,7 @@
         <v>0</v>
       </c>
       <c r="AL9" s="6"/>
-      <c r="AM9" s="540"/>
+      <c r="AM9" s="539"/>
       <c r="AN9" s="142"/>
     </row>
     <row r="10" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10618,7 +10680,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O10" s="673"/>
+      <c r="O10" s="692"/>
       <c r="P10" s="20"/>
       <c r="Q10" s="2" t="s">
         <v>347</v>
@@ -10626,7 +10688,7 @@
       <c r="R10" s="321" t="s">
         <v>74</v>
       </c>
-      <c r="S10" s="532">
+      <c r="S10" s="531">
         <v>1</v>
       </c>
       <c r="T10" s="519">
@@ -10701,7 +10763,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O11" s="673"/>
+      <c r="O11" s="692"/>
       <c r="P11" s="21" t="s">
         <v>342</v>
       </c>
@@ -10709,7 +10771,7 @@
       <c r="R11" s="321" t="s">
         <v>241</v>
       </c>
-      <c r="S11" s="532"/>
+      <c r="S11" s="531"/>
       <c r="T11" s="519">
         <v>2</v>
       </c>
@@ -10757,11 +10819,11 @@
         <v>0</v>
       </c>
       <c r="AL11" s="6"/>
-      <c r="AM11" s="539"/>
+      <c r="AM11" s="538"/>
       <c r="AN11" s="142"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="617" t="s">
+      <c r="A12" s="662" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -10770,11 +10832,11 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="668" t="s">
+      <c r="E12" s="616" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="267"/>
-      <c r="H12" s="546">
+      <c r="H12" s="545">
         <v>-1</v>
       </c>
       <c r="I12" s="61" t="s">
@@ -10791,7 +10853,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O12" s="673"/>
+      <c r="O12" s="692"/>
       <c r="P12" s="21" t="s">
         <v>342</v>
       </c>
@@ -10799,7 +10861,7 @@
       <c r="R12" s="321" t="s">
         <v>240</v>
       </c>
-      <c r="S12" s="532"/>
+      <c r="S12" s="531"/>
       <c r="T12" s="519">
         <v>1</v>
       </c>
@@ -10855,7 +10917,7 @@
       <c r="AL12" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="AM12" s="539" t="s">
+      <c r="AM12" s="538" t="s">
         <v>525</v>
       </c>
       <c r="AN12" s="301" t="s">
@@ -10863,14 +10925,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="619"/>
+      <c r="A13" s="664"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="669"/>
+      <c r="E13" s="617"/>
       <c r="F13" s="176">
         <v>0</v>
       </c>
@@ -10893,7 +10955,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O13" s="673"/>
+      <c r="O13" s="692"/>
       <c r="P13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10901,7 +10963,7 @@
       <c r="R13" s="321" t="s">
         <v>234</v>
       </c>
-      <c r="S13" s="532"/>
+      <c r="S13" s="531"/>
       <c r="T13" s="519">
         <v>2</v>
       </c>
@@ -10949,7 +11011,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="16"/>
-      <c r="AM13" s="539"/>
+      <c r="AM13" s="538"/>
       <c r="AN13" s="142"/>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10963,13 +11025,13 @@
       <c r="K14" s="403"/>
       <c r="L14" s="338"/>
       <c r="M14" s="297">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="299">
         <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="O14" s="673"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="692"/>
       <c r="P14" s="20"/>
       <c r="Q14" s="205" t="s">
         <v>346</v>
@@ -10977,9 +11039,9 @@
       <c r="R14" s="321" t="s">
         <v>246</v>
       </c>
-      <c r="S14" s="532"/>
+      <c r="S14" s="531"/>
       <c r="T14" s="519">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14" s="520">
         <v>-1</v>
@@ -10987,51 +11049,51 @@
       <c r="V14" s="523"/>
       <c r="W14" s="517">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X14" s="302"/>
       <c r="Y14" s="117">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="296">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA14" s="296">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB14" s="296">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="300">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="306"/>
       <c r="AE14" s="302"/>
       <c r="AF14" s="302">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG14" s="348"/>
       <c r="AH14" s="158"/>
       <c r="AI14" s="314">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14" s="315">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK14" s="316">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL14" s="6" t="s">
         <v>577</v>
       </c>
-      <c r="AM14" s="541" t="s">
+      <c r="AM14" s="540" t="s">
         <v>580</v>
       </c>
       <c r="AN14" s="142" t="s">
@@ -11064,7 +11126,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O15" s="673"/>
+      <c r="O15" s="692"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="205" t="s">
         <v>346</v>
@@ -11072,14 +11134,14 @@
       <c r="R15" s="321" t="s">
         <v>232</v>
       </c>
-      <c r="S15" s="532"/>
+      <c r="S15" s="531"/>
       <c r="T15" s="519">
         <v>1</v>
       </c>
       <c r="U15" s="520">
         <v>-2</v>
       </c>
-      <c r="V15" s="531"/>
+      <c r="V15" s="530"/>
       <c r="W15" s="517">
         <f t="shared" si="2"/>
         <v>1</v>
@@ -11130,7 +11192,7 @@
       <c r="AL15" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="AM15" s="539" t="s">
+      <c r="AM15" s="538" t="s">
         <v>466</v>
       </c>
       <c r="AN15" s="142"/>
@@ -11151,7 +11213,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O16" s="673"/>
+      <c r="O16" s="692"/>
       <c r="P16" s="21" t="s">
         <v>342</v>
       </c>
@@ -11161,14 +11223,14 @@
       <c r="R16" s="321" t="s">
         <v>235</v>
       </c>
-      <c r="S16" s="532"/>
+      <c r="S16" s="531"/>
       <c r="T16" s="519">
         <v>2</v>
       </c>
       <c r="U16" s="520">
         <v>-3</v>
       </c>
-      <c r="V16" s="531"/>
+      <c r="V16" s="530"/>
       <c r="W16" s="517">
         <f t="shared" si="2"/>
         <v>1</v>
@@ -11219,7 +11281,7 @@
       <c r="AL16" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="AM16" s="535" t="s">
+      <c r="AM16" s="534" t="s">
         <v>573</v>
       </c>
       <c r="AN16" s="107" t="s">
@@ -11249,7 +11311,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O17" s="673"/>
+      <c r="O17" s="692"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="2" t="s">
         <v>348</v>
@@ -11257,7 +11319,7 @@
       <c r="R17" s="321" t="s">
         <v>97</v>
       </c>
-      <c r="S17" s="532">
+      <c r="S17" s="531">
         <v>1</v>
       </c>
       <c r="T17" s="519">
@@ -11313,7 +11375,7 @@
       <c r="AL17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AM17" s="536" t="s">
+      <c r="AM17" s="535" t="s">
         <v>582</v>
       </c>
       <c r="AN17" s="64" t="s">
@@ -11344,7 +11406,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="O18" s="673"/>
+      <c r="O18" s="692"/>
       <c r="P18" s="21" t="s">
         <v>342</v>
       </c>
@@ -11352,7 +11414,7 @@
       <c r="R18" s="321" t="s">
         <v>248</v>
       </c>
-      <c r="S18" s="532"/>
+      <c r="S18" s="531"/>
       <c r="T18" s="519">
         <v>3</v>
       </c>
@@ -11404,7 +11466,7 @@
         <v>0</v>
       </c>
       <c r="AL18" s="6"/>
-      <c r="AM18" s="542"/>
+      <c r="AM18" s="541"/>
       <c r="AN18" s="142"/>
     </row>
     <row r="19" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11427,7 +11489,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O19" s="673"/>
+      <c r="O19" s="692"/>
       <c r="P19" s="20"/>
       <c r="Q19" s="2" t="s">
         <v>341</v>
@@ -11435,7 +11497,7 @@
       <c r="R19" s="321" t="s">
         <v>247</v>
       </c>
-      <c r="S19" s="532"/>
+      <c r="S19" s="531"/>
       <c r="T19" s="519">
         <v>0</v>
       </c>
@@ -11527,22 +11589,22 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="O20" s="674"/>
+      <c r="O20" s="693"/>
       <c r="P20" s="564" t="s">
         <v>342</v>
       </c>
-      <c r="Q20" s="670"/>
+      <c r="Q20" s="618"/>
       <c r="R20" s="321" t="s">
         <v>86</v>
       </c>
-      <c r="S20" s="532"/>
+      <c r="S20" s="531"/>
       <c r="T20" s="519">
         <v>1</v>
       </c>
       <c r="U20" s="520">
         <v>-3</v>
       </c>
-      <c r="V20" s="533"/>
+      <c r="V20" s="532"/>
       <c r="W20" s="517">
         <f t="shared" si="2"/>
         <v>2</v>
@@ -11589,7 +11651,7 @@
       <c r="AL20" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AM20" s="539" t="s">
+      <c r="AM20" s="538" t="s">
         <v>462</v>
       </c>
     </row>
@@ -11626,7 +11688,7 @@
       <c r="R21" s="321" t="s">
         <v>250</v>
       </c>
-      <c r="S21" s="532">
+      <c r="S21" s="531">
         <v>1</v>
       </c>
       <c r="T21" s="519">
@@ -11686,7 +11748,7 @@
       <c r="AL21" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AM21" s="539" t="s">
+      <c r="AM21" s="538" t="s">
         <v>462</v>
       </c>
       <c r="AN21" s="142"/>
@@ -11709,14 +11771,14 @@
       <c r="R22" s="321" t="s">
         <v>265</v>
       </c>
-      <c r="S22" s="532"/>
+      <c r="S22" s="531"/>
       <c r="T22" s="519">
         <v>2</v>
       </c>
       <c r="U22" s="520">
         <v>-2</v>
       </c>
-      <c r="V22" s="533"/>
+      <c r="V22" s="532"/>
       <c r="W22" s="517">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -11763,11 +11825,11 @@
         <v>0</v>
       </c>
       <c r="AL22" s="16"/>
-      <c r="AM22" s="542"/>
+      <c r="AM22" s="541"/>
       <c r="AN22" s="142"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="624" t="s">
+      <c r="E23" s="669" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="184"/>
@@ -11794,7 +11856,7 @@
       <c r="R23" s="321" t="s">
         <v>252</v>
       </c>
-      <c r="S23" s="532"/>
+      <c r="S23" s="531"/>
       <c r="T23" s="519">
         <v>1</v>
       </c>
@@ -11852,7 +11914,7 @@
       <c r="AL23" s="6" t="s">
         <v>586</v>
       </c>
-      <c r="AM23" s="539" t="s">
+      <c r="AM23" s="538" t="s">
         <v>583</v>
       </c>
       <c r="AN23" s="142" t="s">
@@ -11863,7 +11925,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="625"/>
+      <c r="E24" s="670"/>
       <c r="F24" s="176"/>
       <c r="H24" s="42">
         <v>-1</v>
@@ -11884,11 +11946,11 @@
       <c r="P24" s="564" t="s">
         <v>342</v>
       </c>
-      <c r="Q24" s="670"/>
+      <c r="Q24" s="618"/>
       <c r="R24" s="321" t="s">
         <v>254</v>
       </c>
-      <c r="S24" s="532">
+      <c r="S24" s="531">
         <v>1</v>
       </c>
       <c r="T24" s="519">
@@ -11897,7 +11959,7 @@
       <c r="U24" s="520">
         <v>-2</v>
       </c>
-      <c r="V24" s="531"/>
+      <c r="V24" s="530"/>
       <c r="W24" s="517">
         <f t="shared" si="2"/>
         <v>2</v>
@@ -11948,7 +12010,7 @@
       <c r="AL24" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="AM24" s="545" t="s">
+      <c r="AM24" s="544" t="s">
         <v>342</v>
       </c>
       <c r="AN24" s="142" t="s">
@@ -11980,7 +12042,7 @@
       <c r="R25" s="321" t="s">
         <v>255</v>
       </c>
-      <c r="S25" s="532">
+      <c r="S25" s="531">
         <v>2</v>
       </c>
       <c r="T25" s="519">
@@ -11989,7 +12051,7 @@
       <c r="U25" s="520">
         <v>-2</v>
       </c>
-      <c r="V25" s="533"/>
+      <c r="V25" s="532"/>
       <c r="W25" s="517">
         <f t="shared" si="2"/>
         <v>1</v>
@@ -12034,7 +12096,7 @@
       <c r="AL25" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="AM25" s="539" t="s">
+      <c r="AM25" s="538" t="s">
         <v>468</v>
       </c>
       <c r="AN25" s="142"/>
@@ -12067,7 +12129,7 @@
       <c r="R26" s="321" t="s">
         <v>256</v>
       </c>
-      <c r="S26" s="532">
+      <c r="S26" s="531">
         <v>1</v>
       </c>
       <c r="T26" s="519">
@@ -12122,10 +12184,10 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="AL26" s="746" t="s">
+      <c r="AL26" s="553" t="s">
         <v>256</v>
       </c>
-      <c r="AM26" s="539" t="s">
+      <c r="AM26" s="538" t="s">
         <v>615</v>
       </c>
       <c r="AN26" s="142"/>
@@ -12154,7 +12216,7 @@
       <c r="R27" s="321" t="s">
         <v>257</v>
       </c>
-      <c r="S27" s="532">
+      <c r="S27" s="531">
         <v>2</v>
       </c>
       <c r="T27" s="519">
@@ -12163,7 +12225,7 @@
       <c r="U27" s="520">
         <v>-2</v>
       </c>
-      <c r="V27" s="531"/>
+      <c r="V27" s="530"/>
       <c r="W27" s="517">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -12204,7 +12266,7 @@
         <v>0</v>
       </c>
       <c r="AL27" s="16"/>
-      <c r="AM27" s="542"/>
+      <c r="AM27" s="541"/>
       <c r="AN27" s="142"/>
     </row>
     <row r="28" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12223,14 +12285,14 @@
       <c r="R28" s="321" t="s">
         <v>253</v>
       </c>
-      <c r="S28" s="532"/>
+      <c r="S28" s="531"/>
       <c r="T28" s="519">
         <v>1</v>
       </c>
       <c r="U28" s="520">
         <v>-1</v>
       </c>
-      <c r="V28" s="531"/>
+      <c r="V28" s="530"/>
       <c r="W28" s="517">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -12270,7 +12332,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM28" s="542"/>
+      <c r="AM28" s="541"/>
       <c r="AN28" s="142"/>
     </row>
     <row r="29" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12299,10 +12361,10 @@
         <v>266</v>
       </c>
       <c r="S29" s="518"/>
-      <c r="T29" s="526">
+      <c r="T29" s="525">
         <v>2</v>
       </c>
-      <c r="U29" s="527">
+      <c r="U29" s="526">
         <v>-2</v>
       </c>
       <c r="V29" s="521"/>
@@ -12349,7 +12411,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM29" s="542"/>
+      <c r="AM29" s="541"/>
       <c r="AN29" s="142"/>
     </row>
     <row r="30" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12406,7 +12468,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM30" s="542"/>
+      <c r="AM30" s="541"/>
       <c r="AN30" s="142"/>
     </row>
     <row r="31" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12419,7 +12481,7 @@
       <c r="F31" s="100">
         <v>-1</v>
       </c>
-      <c r="H31" s="546">
+      <c r="H31" s="545">
         <v>-1</v>
       </c>
       <c r="I31" s="21" t="s">
@@ -12477,19 +12539,19 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AM31" s="542"/>
+      <c r="AM31" s="541"/>
       <c r="AN31" s="142"/>
     </row>
     <row r="32" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>-1</v>
       </c>
-      <c r="I32" s="620" t="s">
+      <c r="I32" s="665" t="s">
         <v>606</v>
       </c>
-      <c r="J32" s="671"/>
+      <c r="J32" s="690"/>
       <c r="K32" s="406"/>
-      <c r="L32" s="543">
+      <c r="L32" s="542">
         <v>0</v>
       </c>
       <c r="M32" s="255">
@@ -12565,7 +12627,7 @@
       <c r="AL32" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="AM32" s="539" t="s">
+      <c r="AM32" s="538" t="s">
         <v>465</v>
       </c>
       <c r="AN32" s="107" t="s">
@@ -12635,7 +12697,7 @@
         <v>0</v>
       </c>
       <c r="AL33" s="6"/>
-      <c r="AM33" s="542"/>
+      <c r="AM33" s="541"/>
       <c r="AN33" s="142"/>
     </row>
     <row r="34" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12705,7 +12767,9 @@
         <v>2</v>
       </c>
       <c r="AG34" s="348"/>
-      <c r="AH34" s="326"/>
+      <c r="AH34" s="326">
+        <v>1</v>
+      </c>
       <c r="AI34" s="347">
         <f t="shared" si="7"/>
         <v>2</v>
@@ -12721,7 +12785,7 @@
       <c r="AL34" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="AM34" s="539" t="s">
+      <c r="AM34" s="538" t="s">
         <v>583</v>
       </c>
       <c r="AN34" s="142" t="s">
@@ -12803,7 +12867,7 @@
       <c r="AL35" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="AM35" s="539"/>
+      <c r="AM35" s="538"/>
       <c r="AN35" s="142"/>
     </row>
     <row r="36" spans="2:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12821,7 +12885,7 @@
       <c r="M36" s="255">
         <v>0</v>
       </c>
-      <c r="N36" s="553">
+      <c r="N36" s="552">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -12880,7 +12944,7 @@
       <c r="AL36" s="6" t="s">
         <v>313</v>
       </c>
-      <c r="AM36" s="542"/>
+      <c r="AM36" s="541"/>
       <c r="AN36" s="142" t="s">
         <v>584</v>
       </c>
@@ -12895,7 +12959,7 @@
       <c r="E37" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="H37" s="546">
+      <c r="H37" s="545">
         <v>-1</v>
       </c>
       <c r="K37" s="405" t="s">
@@ -12973,7 +13037,7 @@
       <c r="AL37" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="AM37" s="536" t="s">
+      <c r="AM37" s="535" t="s">
         <v>582</v>
       </c>
       <c r="AN37" s="107" t="s">
@@ -12982,6 +13046,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="O4:O20"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
@@ -12991,13 +13062,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="U2:U3"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="O4:O20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13035,12 +13099,12 @@
       <c r="B1" s="564" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="670"/>
+      <c r="C1" s="618"/>
       <c r="D1" s="209"/>
       <c r="J1" s="564" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="670"/>
+      <c r="K1" s="618"/>
       <c r="L1" s="200" t="s">
         <v>337</v>
       </c>
@@ -13431,7 +13495,7 @@
       <c r="V1" s="564" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="670"/>
+      <c r="W1" s="618"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -13450,7 +13514,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="714" t="s">
+      <c r="AD1" s="707" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -13467,10 +13531,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="745" t="s">
+      <c r="F2" s="706" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="702" t="s">
+      <c r="G2" s="734" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -13498,10 +13562,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="678" t="s">
+      <c r="V2" s="674" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="679"/>
+      <c r="W2" s="675"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -13520,7 +13584,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="715"/>
+      <c r="AD2" s="708"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -13539,8 +13603,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="621"/>
-      <c r="G3" s="703"/>
+      <c r="F3" s="666"/>
+      <c r="G3" s="735"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -13551,13 +13615,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="712" t="s">
+      <c r="O3" s="744" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="733" t="s">
+      <c r="P3" s="726" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="734"/>
+      <c r="Q3" s="727"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -13567,15 +13631,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="715"/>
+      <c r="AD3" s="708"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="703"/>
+      <c r="G4" s="735"/>
       <c r="H4" s="6"/>
       <c r="L4" s="697" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="713"/>
+      <c r="O4" s="745"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -13589,8 +13653,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="566"/>
-      <c r="AA4" s="670"/>
-      <c r="AD4" s="715"/>
+      <c r="AA4" s="618"/>
+      <c r="AD4" s="708"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -13605,21 +13669,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="703"/>
+      <c r="G5" s="735"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="720" t="s">
+      <c r="K5" s="713" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="735"/>
+      <c r="L5" s="728"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="713"/>
+      <c r="O5" s="745"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -13635,11 +13699,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="723" t="s">
+      <c r="Y5" s="716" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="724"/>
-      <c r="AD5" s="715"/>
+      <c r="Z5" s="717"/>
+      <c r="AD5" s="708"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -13649,16 +13713,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="703"/>
+      <c r="G6" s="735"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="721"/>
-      <c r="L6" s="735"/>
-      <c r="O6" s="713"/>
+      <c r="K6" s="714"/>
+      <c r="L6" s="728"/>
+      <c r="O6" s="745"/>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -13668,23 +13732,23 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="715"/>
+      <c r="AD6" s="708"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="703"/>
+      <c r="G7" s="735"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="721"/>
-      <c r="L7" s="735"/>
+      <c r="K7" s="714"/>
+      <c r="L7" s="728"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="713"/>
+      <c r="O7" s="745"/>
       <c r="P7" s="73"/>
       <c r="U7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="715"/>
+      <c r="AD7" s="708"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -13697,7 +13761,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="703"/>
+      <c r="G8" s="735"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -13707,41 +13771,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="721"/>
-      <c r="L8" s="735"/>
-      <c r="O8" s="713"/>
+      <c r="K8" s="714"/>
+      <c r="L8" s="728"/>
+      <c r="O8" s="745"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="717" t="s">
+      <c r="S8" s="710" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="718"/>
-      <c r="U8" s="718"/>
-      <c r="V8" s="718"/>
-      <c r="W8" s="718"/>
-      <c r="X8" s="718"/>
-      <c r="Y8" s="718"/>
-      <c r="Z8" s="718"/>
-      <c r="AA8" s="718"/>
-      <c r="AB8" s="718"/>
-      <c r="AC8" s="719"/>
-      <c r="AD8" s="715"/>
+      <c r="T8" s="711"/>
+      <c r="U8" s="711"/>
+      <c r="V8" s="711"/>
+      <c r="W8" s="711"/>
+      <c r="X8" s="711"/>
+      <c r="Y8" s="711"/>
+      <c r="Z8" s="711"/>
+      <c r="AA8" s="711"/>
+      <c r="AB8" s="711"/>
+      <c r="AC8" s="712"/>
+      <c r="AD8" s="708"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="739"/>
-      <c r="G9" s="703"/>
+      <c r="C9" s="700"/>
+      <c r="G9" s="735"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="721"/>
-      <c r="L9" s="706" t="s">
+      <c r="K9" s="714"/>
+      <c r="L9" s="738" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="707"/>
-      <c r="N9" s="708"/>
-      <c r="O9" s="713"/>
+      <c r="M9" s="739"/>
+      <c r="N9" s="740"/>
+      <c r="O9" s="745"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="715"/>
+      <c r="AD9" s="708"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="740"/>
+      <c r="C10" s="701"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -13749,7 +13813,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="703"/>
+      <c r="G10" s="735"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -13757,33 +13821,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="721"/>
-      <c r="M10" s="742" t="s">
+      <c r="K10" s="714"/>
+      <c r="M10" s="703" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="743"/>
-      <c r="O10" s="743"/>
-      <c r="P10" s="743"/>
-      <c r="Q10" s="743"/>
-      <c r="R10" s="743"/>
-      <c r="S10" s="743"/>
-      <c r="T10" s="743"/>
-      <c r="U10" s="743"/>
-      <c r="V10" s="743"/>
-      <c r="W10" s="743"/>
-      <c r="X10" s="743"/>
-      <c r="Y10" s="743"/>
-      <c r="Z10" s="743"/>
-      <c r="AA10" s="743"/>
-      <c r="AB10" s="743"/>
-      <c r="AC10" s="744"/>
-      <c r="AD10" s="715"/>
+      <c r="N10" s="704"/>
+      <c r="O10" s="704"/>
+      <c r="P10" s="704"/>
+      <c r="Q10" s="704"/>
+      <c r="R10" s="704"/>
+      <c r="S10" s="704"/>
+      <c r="T10" s="704"/>
+      <c r="U10" s="704"/>
+      <c r="V10" s="704"/>
+      <c r="W10" s="704"/>
+      <c r="X10" s="704"/>
+      <c r="Y10" s="704"/>
+      <c r="Z10" s="704"/>
+      <c r="AA10" s="704"/>
+      <c r="AB10" s="704"/>
+      <c r="AC10" s="705"/>
+      <c r="AD10" s="708"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="741"/>
-      <c r="G11" s="703"/>
+      <c r="C11" s="702"/>
+      <c r="G11" s="735"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="721"/>
+      <c r="K11" s="714"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -13791,17 +13855,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="731" t="s">
+      <c r="Z11" s="724" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="732"/>
+      <c r="AA11" s="725"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="715"/>
+      <c r="AD11" s="708"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -13814,7 +13878,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="703"/>
+      <c r="G12" s="735"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -13822,8 +13886,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="721"/>
-      <c r="L12" s="736" t="s">
+      <c r="K12" s="714"/>
+      <c r="L12" s="729" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -13854,25 +13918,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="725" t="s">
+      <c r="AA12" s="718" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="726"/>
+      <c r="AB12" s="719"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="715"/>
+      <c r="AD12" s="708"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="739"/>
-      <c r="G13" s="703"/>
-      <c r="K13" s="721"/>
-      <c r="L13" s="737"/>
+      <c r="C13" s="700"/>
+      <c r="G13" s="735"/>
+      <c r="K13" s="714"/>
+      <c r="L13" s="730"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="705" t="s">
+      <c r="Q13" s="737" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="630"/>
+      <c r="R13" s="633"/>
       <c r="S13" s="560"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -13881,17 +13945,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="727"/>
-      <c r="AB13" s="728"/>
-      <c r="AD13" s="715"/>
+      <c r="AA13" s="720"/>
+      <c r="AB13" s="721"/>
+      <c r="AD13" s="708"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="741"/>
+      <c r="C14" s="702"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="703"/>
+      <c r="G14" s="735"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -13899,8 +13963,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="721"/>
-      <c r="L14" s="737"/>
+      <c r="K14" s="714"/>
+      <c r="L14" s="730"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -13921,9 +13985,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="727"/>
-      <c r="AB14" s="728"/>
-      <c r="AD14" s="715"/>
+      <c r="AA14" s="720"/>
+      <c r="AB14" s="721"/>
+      <c r="AD14" s="708"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -13938,19 +14002,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="703"/>
+      <c r="G15" s="735"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="721"/>
-      <c r="L15" s="738"/>
-      <c r="Q15" s="705" t="s">
+      <c r="K15" s="714"/>
+      <c r="L15" s="731"/>
+      <c r="Q15" s="737" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="630"/>
+      <c r="R15" s="633"/>
       <c r="S15" s="560"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -13959,14 +14023,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="727"/>
-      <c r="AB15" s="728"/>
-      <c r="AD15" s="715"/>
+      <c r="AA15" s="720"/>
+      <c r="AB15" s="721"/>
+      <c r="AD15" s="708"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="703"/>
-      <c r="K16" s="721"/>
+      <c r="G16" s="735"/>
+      <c r="K16" s="714"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13985,24 +14049,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="727"/>
-      <c r="AB16" s="728"/>
-      <c r="AD16" s="715"/>
+      <c r="AA16" s="720"/>
+      <c r="AB16" s="721"/>
+      <c r="AD16" s="708"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="700" t="s">
+      <c r="F17" s="732" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="703"/>
+      <c r="G17" s="735"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="721"/>
+      <c r="K17" s="714"/>
       <c r="S17" s="560"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -14010,9 +14074,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="727"/>
-      <c r="AB17" s="728"/>
-      <c r="AD17" s="715"/>
+      <c r="AA17" s="720"/>
+      <c r="AB17" s="721"/>
+      <c r="AD17" s="708"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -14022,15 +14086,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="701"/>
-      <c r="G18" s="703"/>
+      <c r="F18" s="733"/>
+      <c r="G18" s="735"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="721"/>
+      <c r="K18" s="714"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -14041,39 +14105,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="729"/>
-      <c r="AB18" s="730"/>
-      <c r="AD18" s="715"/>
+      <c r="AA18" s="722"/>
+      <c r="AB18" s="723"/>
+      <c r="AD18" s="708"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="704"/>
-      <c r="K19" s="722"/>
+      <c r="G19" s="736"/>
+      <c r="K19" s="715"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="709" t="s">
+      <c r="R19" s="741" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="710"/>
-      <c r="T19" s="711"/>
+      <c r="S19" s="742"/>
+      <c r="T19" s="743"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="716"/>
+      <c r="AD19" s="709"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -14085,14 +14152,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>